<commit_message>
przepisanie wydatków sprzed budowy
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -14,8 +14,8 @@
     <sheet name="Plan 1. Transza" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Wydatki budowa'!$M$2:$M$8</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="1">'Wydatki budowa'!$M$2:$M$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Wydatki budowa'!$M$2:$M$9</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="1">'Wydatki budowa'!$M$2:$M$6</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -27,7 +27,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0">
+    <comment ref="E28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="181">
   <si>
     <t>Data</t>
   </si>
@@ -493,13 +493,121 @@
   </si>
   <si>
     <t>5337/T/08/2013</t>
+  </si>
+  <si>
+    <t>Wynaghrodzenie Bory</t>
+  </si>
+  <si>
+    <t>Komin</t>
+  </si>
+  <si>
+    <t>5433/T/08/2013</t>
+  </si>
+  <si>
+    <t>Kanalizacja</t>
+  </si>
+  <si>
+    <t>4765/T/08/2013</t>
+  </si>
+  <si>
+    <t>Projekt</t>
+  </si>
+  <si>
+    <t>Archipelag</t>
+  </si>
+  <si>
+    <t>Zakup projektu</t>
+  </si>
+  <si>
+    <t>Wrocław</t>
+  </si>
+  <si>
+    <t>Marek Glapa</t>
+  </si>
+  <si>
+    <t>Wynagrodzenie architekta</t>
+  </si>
+  <si>
+    <t>Wynagrodzenie kierownika budowy</t>
+  </si>
+  <si>
+    <t>ZDiUK</t>
+  </si>
+  <si>
+    <t>Uzgodnienia</t>
+  </si>
+  <si>
+    <t>Tauron</t>
+  </si>
+  <si>
+    <t>Umowa</t>
+  </si>
+  <si>
+    <t>Elektryk</t>
+  </si>
+  <si>
+    <t>Skrzynka Taurona</t>
+  </si>
+  <si>
+    <t>Koszty kredytu</t>
+  </si>
+  <si>
+    <t>Sąd</t>
+  </si>
+  <si>
+    <t>Danuta Fabrowicz</t>
+  </si>
+  <si>
+    <t>Urząd Skarbowy</t>
+  </si>
+  <si>
+    <t>Tomasz Partyka</t>
+  </si>
+  <si>
+    <t>Projekty przyłączy</t>
+  </si>
+  <si>
+    <t>Operator Koparki</t>
+  </si>
+  <si>
+    <t>ZGK</t>
+  </si>
+  <si>
+    <t>Opłata do ZGK za ponowne uzgodnienie</t>
+  </si>
+  <si>
+    <t>Bory</t>
+  </si>
+  <si>
+    <t>Wynagrodzenie Borek</t>
+  </si>
+  <si>
+    <t>Wniosek o wpis do hipoteki</t>
+  </si>
+  <si>
+    <t>0. Przed budową</t>
+  </si>
+  <si>
+    <t>1. Fundamenty</t>
+  </si>
+  <si>
+    <t>2. Ściany nadziemia</t>
+  </si>
+  <si>
+    <t>3. Stropy, schody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marek  </t>
+  </si>
+  <si>
+    <t>Wnioski o wpis do hipotek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +670,33 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Czcionka tekstu podstawowego"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFC00000"/>
+      <name val="Czcionka tekstu podstawowego"/>
     </font>
   </fonts>
   <fills count="18">
@@ -735,17 +870,6 @@
         <color theme="0"/>
       </right>
       <top/>
-      <bottom style="thick">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
@@ -775,11 +899,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -838,8 +971,7 @@
     <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -911,13 +1043,27 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
     <dxf>
       <font>
         <b/>
@@ -930,7 +1076,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="13"/>
-        <color theme="3"/>
+        <color rgb="FFC00000"/>
         <name val="Czcionka tekstu podstawowego"/>
         <scheme val="none"/>
       </font>
@@ -952,6 +1098,22 @@
     <dxf>
       <font>
         <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1262,6 +1424,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1438,25 +1601,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51927680"/>
-        <c:axId val="62602240"/>
+        <c:axId val="62544512"/>
+        <c:axId val="62566784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51927680"/>
+        <c:axId val="62544512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62602240"/>
+        <c:crossAx val="62566784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62602240"/>
+        <c:axId val="62566784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,20 +1628,21 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51927680"/>
+        <c:crossAx val="62544512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1520,24 +1684,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J29" totalsRowCount="1">
-  <autoFilter ref="A1:J28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J53" totalsRowCount="1">
+  <autoFilter ref="A1:J52">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
     <filterColumn colId="3"/>
     <filterColumn colId="7"/>
   </autoFilter>
+  <sortState ref="A2:J52">
+    <sortCondition ref="A1:A52"/>
+  </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="9"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="8"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="7"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="4"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="3"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Zapłacono" totalsRowDxfId="1"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" totalsRowDxfId="0"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="11"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="10"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="9"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" totalsRowDxfId="7"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="6"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="5"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="2" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1553,7 +1720,7 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="10">
+    <tableColumn id="4" name="Plan suma" dataDxfId="12">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+E2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Rzecz suma"/>
@@ -1849,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2281,16 +2448,28 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
+      <c r="A25" s="7">
+        <v>41515</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="9">
+        <v>450</v>
+      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="7">
+        <v>41509</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" s="9">
+        <v>260</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
     </row>
@@ -2367,24 +2546,25 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="135" customWidth="1"/>
+    <col min="10" max="10" width="11" style="133" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" customWidth="1"/>
@@ -2392,14 +2572,14 @@
     <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="125" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="55" t="s">
         <v>121</v>
       </c>
       <c r="D1" t="s">
@@ -2417,692 +2597,1281 @@
       <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="135" t="s">
         <v>136</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="133" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickTop="1">
-      <c r="A2" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="13">
-        <v>1510.21</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="12">
-        <v>41494</v>
-      </c>
-      <c r="H2" s="12">
-        <v>41497</v>
-      </c>
-      <c r="I2" s="12">
-        <v>41495</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="58" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="129">
+        <v>2252</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="136">
+        <v>41015</v>
+      </c>
+      <c r="J2" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="M2" s="57" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="13">
-        <v>5878.78</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="12">
-        <v>41494</v>
-      </c>
-      <c r="H3" s="12">
-        <v>41501</v>
-      </c>
-      <c r="I3" s="12">
-        <v>41501</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>43</v>
+      <c r="A3" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="129">
+        <v>650</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="136">
+        <v>41100</v>
+      </c>
+      <c r="J3" s="133" t="s">
+        <v>117</v>
       </c>
       <c r="L3" t="s">
         <v>119</v>
       </c>
-      <c r="M3" s="124" t="s">
-        <v>76</v>
+      <c r="M3" s="131" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="13">
-        <v>19.079999999999998</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="12">
-        <v>41498</v>
-      </c>
-      <c r="H4" s="12">
-        <v>41501</v>
-      </c>
-      <c r="I4" s="12">
-        <v>41501</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>43</v>
+      <c r="A4" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="129">
+        <v>2800</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="136">
+        <v>41197</v>
+      </c>
+      <c r="J4" s="133" t="s">
+        <v>117</v>
       </c>
       <c r="L4" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="125" t="s">
-        <v>79</v>
+      <c r="M4" s="131" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="13">
-        <v>115.01</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="12">
-        <v>41498</v>
-      </c>
-      <c r="H5" s="12">
-        <v>41501</v>
-      </c>
-      <c r="I5" s="12">
-        <v>41501</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>43</v>
+      <c r="A5" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="129">
+        <v>3000</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="136">
+        <v>41351</v>
+      </c>
+      <c r="J5" s="133" t="s">
+        <v>117</v>
       </c>
       <c r="L5" t="s">
         <v>120</v>
       </c>
-      <c r="M5" s="125" t="s">
-        <v>131</v>
+      <c r="M5" s="132" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="57" t="s">
+      <c r="A6" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="129">
+        <v>148</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="136">
+        <v>41351</v>
+      </c>
+      <c r="J6" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M6" s="132" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="126" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="129">
+        <v>2142</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="136">
+        <v>41352</v>
+      </c>
+      <c r="J7" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="123" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="130">
+        <v>400</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="136">
+        <v>41353</v>
+      </c>
+      <c r="J8" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M8" s="123" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="130">
+        <v>260</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="136">
+        <v>41360</v>
+      </c>
+      <c r="J9" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M9" s="123" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="130">
+        <v>600</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="136">
+        <v>41362</v>
+      </c>
+      <c r="J10" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M10" s="123" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="127" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="130">
+        <v>416</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="136">
+        <v>41367</v>
+      </c>
+      <c r="J11" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M11" s="123" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="127" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="129">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="136">
+        <v>41372</v>
+      </c>
+      <c r="J12" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M12" s="123" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="130">
+        <v>1000</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="136">
+        <v>41382</v>
+      </c>
+      <c r="J13" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M13" s="123" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="22">
+        <v>150</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="136">
+        <v>41391</v>
+      </c>
+      <c r="J14" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="123" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C15" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="127" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="22">
+        <v>200</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="136">
+        <v>41404</v>
+      </c>
+      <c r="J15" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M15" s="123" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="127" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="22">
+        <v>140</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="136">
+        <v>41406</v>
+      </c>
+      <c r="J16" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M16" s="123" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="127" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="22">
+        <v>200</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="136">
+        <v>41428</v>
+      </c>
+      <c r="J17" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M17" s="123" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" s="127" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="22">
+        <v>200</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="136">
+        <v>41484</v>
+      </c>
+      <c r="J18" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="M18" s="123" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="22">
+        <v>147</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="136">
+        <v>41488</v>
+      </c>
+      <c r="J19" s="133" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E20" s="128">
+        <v>450</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="136">
+        <v>41515</v>
+      </c>
+      <c r="J20" s="133" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" s="128">
+        <v>260</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="136">
+        <v>41509</v>
+      </c>
+      <c r="J21" s="133" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="13">
+        <v>1510.21</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="12">
+        <v>41494</v>
+      </c>
+      <c r="H22" s="12">
+        <v>41497</v>
+      </c>
+      <c r="I22" s="137">
+        <v>41495</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="13">
+        <v>5878.78</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="12">
+        <v>41494</v>
+      </c>
+      <c r="H23" s="12">
+        <v>41501</v>
+      </c>
+      <c r="I23" s="137">
+        <v>41501</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="13">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="12">
+        <v>41498</v>
+      </c>
+      <c r="H24" s="12">
+        <v>41501</v>
+      </c>
+      <c r="I24" s="137">
+        <v>41501</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="13">
+        <v>115.01</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="12">
+        <v>41498</v>
+      </c>
+      <c r="H25" s="12">
+        <v>41501</v>
+      </c>
+      <c r="I25" s="137">
+        <v>41501</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B26" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E26" s="13">
         <v>8280.36</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G26" s="12">
         <v>41499</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H26" s="12">
         <v>41502</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I26" s="137">
         <v>41501</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J26" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="125" t="s">
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27">
+        <v>1657.43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="11">
+        <v>41502</v>
+      </c>
+      <c r="H27" s="11">
+        <v>41505</v>
+      </c>
+      <c r="I27" s="137">
+        <v>41502</v>
+      </c>
+      <c r="J27" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="13">
+        <v>512.29999999999995</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="12">
+        <v>41502</v>
+      </c>
+      <c r="H28" s="12">
+        <v>41509</v>
+      </c>
+      <c r="I28" s="137">
+        <v>41507</v>
+      </c>
+      <c r="J28" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29">
+        <v>10584</v>
+      </c>
+      <c r="I29" s="137">
+        <v>41507</v>
+      </c>
+      <c r="J29" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30">
+        <v>400</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="137">
+        <v>41474</v>
+      </c>
+      <c r="J30" s="133" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31">
+        <v>650</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="137">
+        <v>41474</v>
+      </c>
+      <c r="J31" s="133" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32">
+        <v>7800</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="137">
+        <v>41474</v>
+      </c>
+      <c r="J32" s="133" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33">
+        <v>335</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34">
+        <v>7610.63</v>
+      </c>
+      <c r="F34" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" s="11">
+        <v>41514</v>
+      </c>
+      <c r="H34" s="124">
+        <v>41517</v>
+      </c>
+      <c r="I34" s="137">
+        <v>41515</v>
+      </c>
+      <c r="J34" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35">
+        <v>992.96</v>
+      </c>
+      <c r="F35" t="s">
+        <v>149</v>
+      </c>
+      <c r="G35" s="11">
+        <v>41492</v>
+      </c>
+      <c r="H35" s="11">
+        <v>41495</v>
+      </c>
+      <c r="I35" s="137">
+        <v>41516</v>
+      </c>
+      <c r="J35" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36">
+        <v>7236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37">
+        <v>3078</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B39" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="10">
+        <v>3813.05</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="124">
+        <v>41512</v>
+      </c>
+      <c r="H39" s="124">
+        <v>41519</v>
+      </c>
+      <c r="I39" s="137">
+        <v>41515</v>
+      </c>
+      <c r="J39" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="10">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G40" s="124">
+        <v>41513</v>
+      </c>
+      <c r="H40" s="124">
+        <v>41516</v>
+      </c>
+      <c r="I40" s="137">
+        <v>41515</v>
+      </c>
+      <c r="J40" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="10">
+        <v>649.32000000000005</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" s="124">
+        <v>41513</v>
+      </c>
+      <c r="H41" s="124">
+        <v>41516</v>
+      </c>
+      <c r="I41" s="137">
+        <v>41515</v>
+      </c>
+      <c r="J41" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E42" s="10">
+        <v>3084.07</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G42" s="124">
+        <v>41516</v>
+      </c>
+      <c r="H42" s="124">
+        <v>41307</v>
+      </c>
+      <c r="I42" s="136">
+        <v>41516</v>
+      </c>
+      <c r="J42" s="133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B44" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44">
+        <v>5724</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45">
+        <v>6372</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A53" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59">
+        <f>SUBTOTAL(109,[Kwota])</f>
+        <v>105419.38</v>
+      </c>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="138"/>
+      <c r="J53" s="134">
+        <f>SUBTOTAL(103,[Konto])</f>
         <v>37</v>
       </c>
-      <c r="E7">
-        <v>1657.43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="11">
-        <v>41502</v>
-      </c>
-      <c r="H7" s="11">
-        <v>41505</v>
-      </c>
-      <c r="I7" s="11">
-        <v>41502</v>
-      </c>
-      <c r="J7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="125" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="13">
-        <v>512.29999999999995</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="12">
-        <v>41502</v>
-      </c>
-      <c r="H8" s="12">
-        <v>41509</v>
-      </c>
-      <c r="I8" s="12">
-        <v>41507</v>
-      </c>
-      <c r="J8" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="125" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9">
-        <v>10584</v>
-      </c>
-      <c r="J9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="125" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10">
-        <v>400</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="J10" t="s">
-        <v>117</v>
-      </c>
-      <c r="M10" s="125" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E11">
-        <v>650</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="J11" t="s">
-        <v>117</v>
-      </c>
-      <c r="M11" s="125" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12">
-        <v>7800</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="J12" t="s">
-        <v>117</v>
-      </c>
-      <c r="M12" s="125" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13">
-        <v>335</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="M13" s="125" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14">
-        <v>7610.63</v>
-      </c>
-      <c r="F14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G14" s="11">
-        <v>41514</v>
-      </c>
-      <c r="H14" s="126">
-        <v>41517</v>
-      </c>
-      <c r="I14" s="11">
-        <v>41515</v>
-      </c>
-      <c r="J14" t="s">
-        <v>43</v>
-      </c>
-      <c r="M14" s="125" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="55"/>
-      <c r="B15" s="57"/>
-      <c r="M15" s="125" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="55"/>
-      <c r="B16" s="57"/>
-      <c r="M16" s="125" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17">
-        <v>7236</v>
-      </c>
-      <c r="M17" s="125" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18">
-        <v>10584</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19">
-        <v>3078</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20">
-        <v>2052</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21">
-        <v>5724</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22">
-        <v>6372</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="55"/>
-      <c r="B23" s="57"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="55"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" s="10">
-        <v>3813.05</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" s="126">
-        <v>41512</v>
-      </c>
-      <c r="H25" s="126">
-        <v>41519</v>
-      </c>
-      <c r="I25" s="11">
-        <v>41515</v>
-      </c>
-      <c r="J25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="10">
-        <v>66.180000000000007</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G26" s="126">
-        <v>41513</v>
-      </c>
-      <c r="H26" s="126">
-        <v>41516</v>
-      </c>
-      <c r="I26" s="11">
-        <v>41515</v>
-      </c>
-      <c r="J26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E27" s="10">
-        <v>649.32000000000005</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="G27" s="126">
-        <v>41513</v>
-      </c>
-      <c r="H27" s="126">
-        <v>41516</v>
-      </c>
-      <c r="I27" s="11">
-        <v>41515</v>
-      </c>
-      <c r="J27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="57"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-    </row>
-    <row r="29" spans="1:13" ht="17.25" thickBot="1">
-      <c r="A29" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60">
-        <f>SUBTOTAL(109,[Kwota])</f>
-        <v>84927.349999999991</v>
-      </c>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60">
-        <f>SUBTOTAL(103,[Konto])</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" thickTop="1"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="61" spans="1:10">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="139"/>
+      <c r="J61" s="127"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="139"/>
+      <c r="J78" s="127"/>
+    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A28">
-      <formula1>$M$3:$M$17</formula1>
+  <dataConsolidate/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A54:A61">
+      <formula1>$M$4:$M$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B61 B50:B52 B22:B45">
       <formula1>$L$3:$L$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A52">
+      <formula1>$M$3:$M$18</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3119,7 +3888,7 @@
   <dimension ref="B1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3133,9 +3902,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
@@ -3164,7 +3933,7 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="58">
         <v>0</v>
       </c>
       <c r="F3">
@@ -3181,11 +3950,11 @@
       <c r="D4">
         <v>46700</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E3</f>
         <v>37600</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="58">
         <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
         <v>9100</v>
       </c>
@@ -3197,11 +3966,11 @@
       <c r="C5">
         <v>37800</v>
       </c>
-      <c r="E5" s="59">
+      <c r="E5" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E4</f>
         <v>75400</v>
       </c>
-      <c r="F5" s="59"/>
+      <c r="F5" s="58"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
@@ -3210,11 +3979,11 @@
       <c r="C6">
         <v>43200</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E5</f>
         <v>118600</v>
       </c>
-      <c r="F6" s="59"/>
+      <c r="F6" s="58"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
@@ -3223,11 +3992,11 @@
       <c r="C7">
         <v>47500</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E6</f>
         <v>166100</v>
       </c>
-      <c r="F7" s="59"/>
+      <c r="F7" s="58"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
@@ -3236,11 +4005,11 @@
       <c r="C8">
         <v>32000</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E7</f>
         <v>198100</v>
       </c>
-      <c r="F8" s="59"/>
+      <c r="F8" s="58"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
@@ -3249,11 +4018,11 @@
       <c r="C9">
         <v>21600</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E8</f>
         <v>219700</v>
       </c>
-      <c r="F9" s="59"/>
+      <c r="F9" s="58"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
@@ -3262,7 +4031,7 @@
       <c r="C10">
         <v>9700</v>
       </c>
-      <c r="E10" s="59">
+      <c r="E10" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E9</f>
         <v>229400</v>
       </c>
@@ -3274,7 +4043,7 @@
       <c r="C11">
         <v>45700</v>
       </c>
-      <c r="E11" s="59">
+      <c r="E11" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E10</f>
         <v>275100</v>
       </c>
@@ -3286,7 +4055,7 @@
       <c r="C12">
         <v>16200</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E11</f>
         <v>291300</v>
       </c>
@@ -3298,7 +4067,7 @@
       <c r="C13">
         <v>22200</v>
       </c>
-      <c r="E13" s="59">
+      <c r="E13" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E12</f>
         <v>313500</v>
       </c>
@@ -3310,7 +4079,7 @@
       <c r="C14">
         <v>39900</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E13</f>
         <v>353400</v>
       </c>
@@ -3322,7 +4091,7 @@
       <c r="C15">
         <v>6500</v>
       </c>
-      <c r="E15" s="59">
+      <c r="E15" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E14</f>
         <v>359900</v>
       </c>
@@ -3334,7 +4103,7 @@
       <c r="C16">
         <v>31300</v>
       </c>
-      <c r="E16" s="59">
+      <c r="E16" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E15</f>
         <v>391200</v>
       </c>
@@ -3346,7 +4115,7 @@
       <c r="C17">
         <v>20000</v>
       </c>
-      <c r="E17" s="59">
+      <c r="E17" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E16</f>
         <v>411200</v>
       </c>
@@ -3358,7 +4127,7 @@
       <c r="C18">
         <v>31600</v>
       </c>
-      <c r="E18" s="59">
+      <c r="E18" s="58">
         <f>Tabela5[[#This Row],[Planowane]]+E17</f>
         <v>442800</v>
       </c>
@@ -3428,10 +4197,10 @@
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
       <c r="G2" s="31"/>
-      <c r="J2" s="108" t="s">
+      <c r="J2" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="108">
+      <c r="K2" s="107">
         <v>37600</v>
       </c>
     </row>
@@ -3459,10 +4228,10 @@
         <f>F3-2100</f>
         <v>5900</v>
       </c>
-      <c r="J3" s="109" t="s">
+      <c r="J3" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="109">
+      <c r="K3" s="108">
         <v>37800</v>
       </c>
     </row>
@@ -3487,10 +4256,10 @@
         <v>3200</v>
       </c>
       <c r="G4" s="31"/>
-      <c r="J4" s="110" t="s">
+      <c r="J4" s="109" t="s">
         <v>131</v>
       </c>
-      <c r="K4" s="110">
+      <c r="K4" s="109">
         <v>43200</v>
       </c>
     </row>
@@ -3515,10 +4284,10 @@
         <v>17800</v>
       </c>
       <c r="G5" s="31"/>
-      <c r="J5" s="111" t="s">
+      <c r="J5" s="110" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="111">
+      <c r="K5" s="110">
         <v>47500</v>
       </c>
     </row>
@@ -3539,10 +4308,10 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="31"/>
-      <c r="J6" s="112" t="s">
+      <c r="J6" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="K6" s="112">
+      <c r="K6" s="111">
         <v>32000</v>
       </c>
     </row>
@@ -3567,10 +4336,10 @@
         <v>8600</v>
       </c>
       <c r="G7" s="31"/>
-      <c r="J7" s="113" t="s">
+      <c r="J7" s="112" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="113">
+      <c r="K7" s="112">
         <v>21600</v>
       </c>
     </row>
@@ -3596,64 +4365,64 @@
         <v>12400</v>
       </c>
       <c r="G8" s="48"/>
-      <c r="J8" s="114" t="s">
+      <c r="J8" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="114">
+      <c r="K8" s="113">
         <v>9700</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="66">
+      <c r="A9" s="65">
         <v>8</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="66">
         <v>43200</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="67">
         <f t="shared" si="0"/>
         <v>9.7560975609756101E-2</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="68">
         <f t="shared" ref="E9:E33" si="1">C9-F9</f>
         <v>43200</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
-      <c r="J9" s="115" t="s">
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
+      <c r="J9" s="114" t="s">
         <v>95</v>
       </c>
-      <c r="K9" s="115">
+      <c r="K9" s="114">
         <v>45700</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="88">
+      <c r="A10" s="87">
         <v>9</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="89">
+      <c r="C10" s="88">
         <v>9700</v>
       </c>
-      <c r="D10" s="90">
+      <c r="D10" s="89">
         <f t="shared" si="0"/>
         <v>2.1906052393857272E-2</v>
       </c>
-      <c r="E10" s="91">
+      <c r="E10" s="90">
         <f t="shared" si="1"/>
         <v>9700</v>
       </c>
-      <c r="F10" s="91"/>
-      <c r="G10" s="92"/>
-      <c r="J10" s="116" t="s">
+      <c r="F10" s="90"/>
+      <c r="G10" s="91"/>
+      <c r="J10" s="115" t="s">
         <v>92</v>
       </c>
-      <c r="K10" s="116">
+      <c r="K10" s="115">
         <v>16200</v>
       </c>
     </row>
@@ -3677,10 +4446,10 @@
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="53"/>
-      <c r="J11" s="117" t="s">
+      <c r="J11" s="116" t="s">
         <v>135</v>
       </c>
-      <c r="K11" s="117">
+      <c r="K11" s="116">
         <v>22200</v>
       </c>
     </row>
@@ -3704,37 +4473,37 @@
       </c>
       <c r="F12" s="52"/>
       <c r="G12" s="53"/>
-      <c r="J12" s="118" t="s">
+      <c r="J12" s="117" t="s">
         <v>134</v>
       </c>
-      <c r="K12" s="118">
+      <c r="K12" s="117">
         <v>39900</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="71">
+      <c r="A13" s="70">
         <v>12</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C13" s="71">
         <v>32000</v>
       </c>
-      <c r="D13" s="73">
+      <c r="D13" s="72">
         <f t="shared" si="0"/>
         <v>7.2267389340560068E-2</v>
       </c>
-      <c r="E13" s="74">
+      <c r="E13" s="73">
         <f t="shared" si="1"/>
         <v>32000</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
-      <c r="J13" s="119" t="s">
+      <c r="F13" s="73"/>
+      <c r="G13" s="74"/>
+      <c r="J13" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="122">
+      <c r="K13" s="121">
         <v>6500</v>
       </c>
     </row>
@@ -3758,133 +4527,133 @@
       </c>
       <c r="F14" s="42"/>
       <c r="G14" s="43"/>
-      <c r="J14" s="120" t="s">
+      <c r="J14" s="119" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="76">
+      <c r="K14" s="75">
         <v>31300</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="98">
+      <c r="A15" s="97">
         <v>14</v>
       </c>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="99">
+      <c r="C15" s="98">
         <v>6500</v>
       </c>
-      <c r="D15" s="100">
+      <c r="D15" s="99">
         <f t="shared" si="0"/>
         <v>1.4679313459801264E-2</v>
       </c>
-      <c r="E15" s="101">
+      <c r="E15" s="100">
         <f t="shared" si="1"/>
         <v>6500</v>
       </c>
-      <c r="F15" s="101"/>
-      <c r="G15" s="102"/>
-      <c r="J15" s="121" t="s">
+      <c r="F15" s="100"/>
+      <c r="G15" s="101"/>
+      <c r="J15" s="120" t="s">
         <v>132</v>
       </c>
-      <c r="K15" s="121">
+      <c r="K15" s="120">
         <v>20000</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="93">
+      <c r="A16" s="92">
         <v>15</v>
       </c>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="94">
+      <c r="C16" s="93">
         <v>18900</v>
       </c>
-      <c r="D16" s="95">
+      <c r="D16" s="94">
         <f t="shared" si="0"/>
         <v>4.2682926829268296E-2</v>
       </c>
-      <c r="E16" s="96">
+      <c r="E16" s="95">
         <f t="shared" si="1"/>
         <v>18900</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="97"/>
-      <c r="J16" s="121" t="s">
+      <c r="F16" s="95"/>
+      <c r="G16" s="96"/>
+      <c r="J16" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="K16" s="121">
+      <c r="K16" s="120">
         <v>31600</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="93">
+      <c r="A17" s="92">
         <v>16</v>
       </c>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="94">
+      <c r="C17" s="93">
         <v>3300</v>
       </c>
-      <c r="D17" s="95">
+      <c r="D17" s="94">
         <f t="shared" si="0"/>
         <v>7.4525745257452572E-3</v>
       </c>
-      <c r="E17" s="96">
+      <c r="E17" s="95">
         <f t="shared" si="1"/>
         <v>3300</v>
       </c>
-      <c r="F17" s="96"/>
-      <c r="G17" s="97"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="96"/>
       <c r="K17">
         <f>SUM(K2:K16)</f>
         <v>442800</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="77">
+      <c r="A18" s="76">
         <v>17</v>
       </c>
-      <c r="B18" s="77" t="s">
+      <c r="B18" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="81">
+      <c r="C18" s="80">
         <v>12000</v>
       </c>
-      <c r="D18" s="78">
+      <c r="D18" s="77">
         <f t="shared" si="0"/>
         <v>2.7100271002710029E-2</v>
       </c>
-      <c r="E18" s="79">
+      <c r="E18" s="78">
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
-      <c r="F18" s="79"/>
-      <c r="G18" s="80"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="77">
+      <c r="A19" s="76">
         <v>18</v>
       </c>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="81">
+      <c r="C19" s="80">
         <v>27900</v>
       </c>
-      <c r="D19" s="78">
+      <c r="D19" s="77">
         <f t="shared" si="0"/>
         <v>6.3008130081300809E-2</v>
       </c>
-      <c r="E19" s="79">
+      <c r="E19" s="78">
         <f t="shared" si="1"/>
         <v>27900</v>
       </c>
-      <c r="F19" s="79"/>
-      <c r="G19" s="80"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="10">
@@ -3908,25 +4677,25 @@
       <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="103">
+      <c r="A21" s="102">
         <v>20</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="104">
+      <c r="C21" s="103">
         <v>16200</v>
       </c>
-      <c r="D21" s="105">
+      <c r="D21" s="104">
         <f t="shared" si="0"/>
         <v>3.6585365853658534E-2</v>
       </c>
-      <c r="E21" s="106">
+      <c r="E21" s="105">
         <f t="shared" si="1"/>
         <v>16200</v>
       </c>
-      <c r="F21" s="106"/>
-      <c r="G21" s="107"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="106"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="34">
@@ -3971,128 +4740,128 @@
       <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="82">
+      <c r="A24" s="81">
         <v>23</v>
       </c>
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="83"/>
-      <c r="D24" s="84">
+      <c r="C24" s="82"/>
+      <c r="D24" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="85">
+      <c r="E24" s="84">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F24" s="85"/>
-      <c r="G24" s="86"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="85"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="82" t="s">
+      <c r="A25" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="87">
+      <c r="C25" s="86">
         <v>2700</v>
       </c>
-      <c r="D25" s="84">
+      <c r="D25" s="83">
         <f t="shared" si="0"/>
         <v>6.0975609756097563E-3</v>
       </c>
-      <c r="E25" s="85">
+      <c r="E25" s="84">
         <f t="shared" si="1"/>
         <v>2700</v>
       </c>
-      <c r="F25" s="85"/>
-      <c r="G25" s="86"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="85"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="87">
+      <c r="C26" s="86">
         <v>6700</v>
       </c>
-      <c r="D26" s="84">
+      <c r="D26" s="83">
         <f t="shared" si="0"/>
         <v>1.5130984643179765E-2</v>
       </c>
-      <c r="E26" s="85">
+      <c r="E26" s="84">
         <f t="shared" si="1"/>
         <v>6700</v>
       </c>
-      <c r="F26" s="85"/>
-      <c r="G26" s="86"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="85"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="82" t="s">
+      <c r="B27" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="87">
+      <c r="C27" s="86">
         <v>2200</v>
       </c>
-      <c r="D27" s="84">
+      <c r="D27" s="83">
         <f t="shared" si="0"/>
         <v>4.9683830171635048E-3</v>
       </c>
-      <c r="E27" s="85">
+      <c r="E27" s="84">
         <f t="shared" si="1"/>
         <v>2200</v>
       </c>
-      <c r="F27" s="85"/>
-      <c r="G27" s="86"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="82" t="s">
+      <c r="B28" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="87">
+      <c r="C28" s="86">
         <v>15700</v>
       </c>
-      <c r="D28" s="84">
+      <c r="D28" s="83">
         <f t="shared" si="0"/>
         <v>3.5456187895212286E-2</v>
       </c>
-      <c r="E28" s="85">
+      <c r="E28" s="84">
         <f t="shared" si="1"/>
         <v>15700</v>
       </c>
-      <c r="F28" s="85"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="85"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="82" t="s">
+      <c r="A29" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="82" t="s">
+      <c r="B29" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="87">
+      <c r="C29" s="86">
         <v>18400</v>
       </c>
-      <c r="D29" s="84">
+      <c r="D29" s="83">
         <f t="shared" si="0"/>
         <v>4.1553748870822041E-2</v>
       </c>
-      <c r="E29" s="85">
+      <c r="E29" s="84">
         <f t="shared" si="1"/>
         <v>18400</v>
       </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="85"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="10">
@@ -4158,25 +4927,25 @@
       <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="61">
+      <c r="A33" s="60">
         <v>27</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="62">
+      <c r="C33" s="61">
         <v>51600</v>
       </c>
-      <c r="D33" s="63">
+      <c r="D33" s="62">
         <f t="shared" si="0"/>
         <v>0.11653116531165311</v>
       </c>
-      <c r="E33" s="64">
+      <c r="E33" s="63">
         <f t="shared" si="1"/>
         <v>51600</v>
       </c>
-      <c r="F33" s="64"/>
-      <c r="G33" s="65"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="64"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="10"/>

</xml_diff>

<commit_message>
Tabela przestawna z zestawieniem
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -2,20 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="13020" windowHeight="2895"/>
   </bookViews>
   <sheets>
     <sheet name="Wydatki budowa" sheetId="2" r:id="rId1"/>
-    <sheet name="Etapy budowy" sheetId="9" r:id="rId2"/>
-    <sheet name="Harmonogram DB " sheetId="7" r:id="rId3"/>
+    <sheet name="Zestawienie kosztów" sheetId="11" r:id="rId2"/>
+    <sheet name="Etapy budowy" sheetId="9" r:id="rId3"/>
+    <sheet name="Harmonogram DB " sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Wydatki budowa'!$M$2:$M$9</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="0">'Wydatki budowa'!$M$2:$M$6</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
+  <pivotCaches>
+    <pivotCache cacheId="16" r:id="rId5"/>
+  </pivotCaches>
 </workbook>
 </file>
 
@@ -56,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="169">
   <si>
     <t>Opis</t>
   </si>
@@ -343,9 +347,6 @@
     <t>Zero</t>
   </si>
   <si>
-    <t>Rzecz suma</t>
-  </si>
-  <si>
     <t>Nazwy etapów</t>
   </si>
   <si>
@@ -518,12 +519,63 @@
   </si>
   <si>
     <t>Wpis BZ, wypis KW</t>
+  </si>
+  <si>
+    <t>bez faktury</t>
+  </si>
+  <si>
+    <t>698/2013</t>
+  </si>
+  <si>
+    <t>Zaprawa Nowak</t>
+  </si>
+  <si>
+    <t>F/SK/00799/13</t>
+  </si>
+  <si>
+    <t>9/2013</t>
+  </si>
+  <si>
+    <t>Antoni Nowak</t>
+  </si>
+  <si>
+    <t>Nadproża</t>
+  </si>
+  <si>
+    <t>5441/T/08/2013</t>
+  </si>
+  <si>
+    <t>Rzecz różnica</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Realizacja</t>
+  </si>
+  <si>
+    <t>Etykiety wierszy</t>
+  </si>
+  <si>
+    <t>(puste)</t>
+  </si>
+  <si>
+    <t>Suma końcowa</t>
+  </si>
+  <si>
+    <t>Suma z Kwota</t>
+  </si>
+  <si>
+    <t>Rzeczoznawca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
+  </numFmts>
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -829,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -950,9 +1002,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -962,14 +1011,25 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -1000,11 +1060,6 @@
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1040,13 +1095,33 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <color rgb="FFC00000"/>
+        <sz val="13"/>
+        <color theme="3"/>
+        <name val="Czcionka tekstu podstawowego"/>
+        <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thick">
+          <color theme="4" tint="0.499984740745262"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1064,6 +1139,69 @@
         <name val="Czcionka tekstu podstawowego"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thick">
+          <color theme="4" tint="0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="3"/>
+        <name val="Czcionka tekstu podstawowego"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thick">
+          <color theme="4" tint="0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="3"/>
+        <name val="Czcionka tekstu podstawowego"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1204,97 +1342,29 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="3"/>
-        <name val="Czcionka tekstu podstawowego"/>
-        <scheme val="none"/>
+        <color rgb="FFC00000"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color theme="4" tint="0.499984740745262"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="3"/>
-        <name val="Czcionka tekstu podstawowego"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color theme="4" tint="0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="3"/>
-        <name val="Czcionka tekstu podstawowego"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thick">
-          <color theme="4" tint="0.499984740745262"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1338,7 +1408,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Etapy budowy'!$E$2</c:f>
+              <c:f>'Etapy budowy'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1355,7 +1425,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Etapy budowy'!$B$3:$B$18</c:f>
+              <c:f>'Etapy budowy'!$A$3:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1411,7 +1481,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Etapy budowy'!$E$3:$E$18</c:f>
+              <c:f>'Etapy budowy'!$D$3:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1472,11 +1542,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Etapy budowy'!$F$2</c:f>
+              <c:f>'Etapy budowy'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rzecz suma</c:v>
+                  <c:v>Rzecz różnica</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1489,7 +1559,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Etapy budowy'!$F$3:$F$18</c:f>
+              <c:f>'Etapy budowy'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1504,25 +1574,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63289984"/>
-        <c:axId val="62984576"/>
+        <c:axId val="70915200"/>
+        <c:axId val="70916736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63289984"/>
+        <c:axId val="70915200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62984576"/>
+        <c:crossAx val="70916736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62984576"/>
+        <c:axId val="70916736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1601,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63289984"/>
+        <c:crossAx val="70915200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1545,7 +1615,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1555,16 +1625,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1586,11 +1656,860 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="41523.404467361113" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="53">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabela1"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="Etap" numFmtId="0">
+      <sharedItems containsBlank="1" count="6">
+        <s v="0. Przed budową"/>
+        <s v="1. Fundamenty"/>
+        <s v="2. Ściany nadziemia"/>
+        <s v="3. Stropy, schody"/>
+        <s v="4. Dach"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Typ" numFmtId="0">
+      <sharedItems containsBlank="1" count="6">
+        <s v="Projekt"/>
+        <s v="Usługa"/>
+        <s v="Koszty kredytu"/>
+        <s v="Materiał"/>
+        <s v="Wykonawca"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Dostawca" numFmtId="0">
+      <sharedItems containsBlank="1" count="20">
+        <s v="Archipelag"/>
+        <s v="Wrocław"/>
+        <s v="Marek Glapa"/>
+        <s v="ZDiUK"/>
+        <s v="Tauron"/>
+        <s v="Elektryk"/>
+        <s v="Sąd"/>
+        <s v="Danuta Fabrowicz"/>
+        <s v="Urząd Skarbowy"/>
+        <s v="Rzeczoznawca"/>
+        <s v="Tomasz Partyka"/>
+        <s v="Operator Koparki"/>
+        <s v="Marek  "/>
+        <s v="ZGK"/>
+        <s v="Bory"/>
+        <s v="Manex"/>
+        <s v="Antoni Nowak"/>
+        <s v="Geodeta"/>
+        <s v="Nowak"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Opis" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Kwota" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="19.079999999999998" maxValue="10584"/>
+    </cacheField>
+    <cacheField name="Faktura numer" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Data faktury" numFmtId="0">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-08-06T00:00:00" maxDate="2013-08-31T00:00:00"/>
+    </cacheField>
+    <cacheField name="Data płatności" numFmtId="0">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-08-09T00:00:00" maxDate="2013-09-03T00:00:00"/>
+    </cacheField>
+    <cacheField name="Zapłacono" numFmtId="0">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2012-04-16T00:00:00" maxDate="2013-09-05T00:00:00"/>
+    </cacheField>
+    <cacheField name="Konto" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="53">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Zakup projektu"/>
+    <n v="2252"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2012-04-16T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Mapa do celów projektowych"/>
+    <n v="650"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2012-07-10T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Wynagrodzenie architekta"/>
+    <n v="2800"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2012-10-15T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Wynagrodzenie kierownika budowy"/>
+    <n v="3000"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-03-18T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="Uzgodnienia"/>
+    <n v="148"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-03-18T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Umowa"/>
+    <n v="2142"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-03-19T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Skrzynka Taurona"/>
+    <n v="400"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-03-20T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="6"/>
+    <s v="Wpis BZ, wypis KW"/>
+    <n v="260"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-03-27T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="Projekt płyty fundamentowej"/>
+    <n v="600"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-03-29T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="8"/>
+    <s v="Podatek od umowy najmu"/>
+    <n v="416"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-04-03T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="9"/>
+    <s v="Operaty szacunkowe"/>
+    <n v="1000"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-04-08T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <s v="Projekty przyłączy"/>
+    <n v="1000"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-04-18T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="11"/>
+    <s v="Rozsypanie tłucznia"/>
+    <n v="150"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-04-27T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="12"/>
+    <s v="Siatka leśna"/>
+    <n v="200"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-05-10T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="8"/>
+    <s v="Podatek od umowy najmu"/>
+    <n v="140"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-05-12T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <s v="Partyka - update projektu kanalizacji"/>
+    <n v="200"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-06-03T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <s v="Partyka - update projektu kanalizacji"/>
+    <n v="200"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-07-29T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="13"/>
+    <s v="Opłata do ZGK za ponowne uzgodnienie"/>
+    <n v="147"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-08-02T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="14"/>
+    <s v="Wynagrodzenie Borek"/>
+    <n v="450"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-08-29T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="6"/>
+    <s v="Wniosek o wpis do hipoteki"/>
+    <n v="260"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-08-23T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Folia"/>
+    <n v="1510.21"/>
+    <s v="4817/T/08/2013"/>
+    <d v="2013-08-08T00:00:00"/>
+    <d v="2013-08-11T00:00:00"/>
+    <d v="2013-08-09T00:00:00"/>
+    <s v="mbank dza"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Stal"/>
+    <n v="5878.78"/>
+    <s v="4815/T/08/2013"/>
+    <d v="2013-08-08T00:00:00"/>
+    <d v="2013-08-15T00:00:00"/>
+    <d v="2013-08-15T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Rura woda"/>
+    <n v="19.079999999999998"/>
+    <s v="4877/T/08/2013"/>
+    <d v="2013-08-12T00:00:00"/>
+    <d v="2013-08-15T00:00:00"/>
+    <d v="2013-08-15T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Folia"/>
+    <n v="115.01"/>
+    <s v="4916/T/08/2013"/>
+    <d v="2013-08-12T00:00:00"/>
+    <d v="2013-08-15T00:00:00"/>
+    <d v="2013-08-15T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Styropian"/>
+    <n v="8280.36"/>
+    <s v="4969/T/08/2013"/>
+    <d v="2013-08-13T00:00:00"/>
+    <d v="2013-08-16T00:00:00"/>
+    <d v="2013-08-15T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Stal"/>
+    <n v="1657.43"/>
+    <s v="5017/T/08/2013"/>
+    <d v="2013-08-16T00:00:00"/>
+    <d v="2013-08-19T00:00:00"/>
+    <d v="2013-08-16T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Stal"/>
+    <n v="512.29999999999995"/>
+    <s v="5042/T/08/2013"/>
+    <d v="2013-08-16T00:00:00"/>
+    <d v="2013-08-23T00:00:00"/>
+    <d v="2013-08-21T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Płyta fundamentowa"/>
+    <n v="10584"/>
+    <s v="9/2013"/>
+    <m/>
+    <m/>
+    <d v="2013-08-21T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="Geodeta działka"/>
+    <n v="400"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-07-19T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="Geodeta budynek"/>
+    <n v="650"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-07-19T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="18"/>
+    <s v="Piasek"/>
+    <n v="7800"/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2013-07-19T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="16"/>
+    <s v="Folia Nowak"/>
+    <n v="335.18"/>
+    <s v="698/2013"/>
+    <m/>
+    <m/>
+    <d v="2013-09-04T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Beton"/>
+    <n v="7610.63"/>
+    <s v="5337/T/08/2013"/>
+    <d v="2013-08-28T00:00:00"/>
+    <d v="2013-08-31T00:00:00"/>
+    <d v="2013-08-29T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Kanalizacja"/>
+    <n v="992.96"/>
+    <s v="4765/T/08/2013"/>
+    <d v="2013-08-06T00:00:00"/>
+    <d v="2013-08-09T00:00:00"/>
+    <d v="2013-08-30T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Parter"/>
+    <n v="7010.82"/>
+    <s v="bez faktury"/>
+    <m/>
+    <m/>
+    <d v="2013-09-04T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Ściana kolankowa"/>
+    <n v="3078"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Mur poddasza"/>
+    <n v="2052"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Pustaki"/>
+    <n v="3813.05"/>
+    <s v="5291/T/08/2013"/>
+    <d v="2013-08-26T00:00:00"/>
+    <d v="2013-09-02T00:00:00"/>
+    <d v="2013-08-29T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Smoła"/>
+    <n v="66.180000000000007"/>
+    <s v="5315/T/08/2013"/>
+    <d v="2013-08-27T00:00:00"/>
+    <d v="2013-08-30T00:00:00"/>
+    <d v="2013-08-29T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Pustaki połówki"/>
+    <n v="649.32000000000005"/>
+    <s v="5327/T/08/2013"/>
+    <d v="2013-08-27T00:00:00"/>
+    <d v="2013-08-30T00:00:00"/>
+    <d v="2013-08-29T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Komin"/>
+    <n v="3084.07"/>
+    <s v="5433/T/08/2013"/>
+    <d v="2013-08-30T00:00:00"/>
+    <d v="2013-09-02T00:00:00"/>
+    <d v="2013-08-30T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="16"/>
+    <s v="Zaprawa Nowak"/>
+    <n v="54"/>
+    <s v="F/SK/00799/13"/>
+    <m/>
+    <m/>
+    <d v="2013-09-04T00:00:00"/>
+    <s v="gotówka"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="15"/>
+    <s v="Nadproża"/>
+    <n v="1415.36"/>
+    <s v="5441/T/08/2013"/>
+    <d v="2013-08-30T00:00:00"/>
+    <d v="2013-09-02T00:00:00"/>
+    <d v="2013-09-04T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Strop"/>
+    <n v="10584"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Więźba"/>
+    <n v="5724"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Dach"/>
+    <n v="6372"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="21">
+        <item x="16"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="17"/>
+        <item x="15"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="18"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="13"/>
+        <item x="19"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J53" totalsRowCount="1">
-  <autoFilter ref="A1:J52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J55" totalsRowCount="1">
+  <autoFilter ref="A1:J54">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
+    <filterColumn colId="2"/>
     <filterColumn colId="3"/>
     <filterColumn colId="7"/>
     <filterColumn colId="8"/>
@@ -1599,35 +2518,39 @@
     <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="12"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="11"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="10"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="9"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" totalsRowDxfId="8"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="7"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="6"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="5"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="9"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="8"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="7"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="4"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="3"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="13" totalsRowDxfId="1"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="B2:F18" totalsRowShown="0">
-  <autoFilter ref="B2:F18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A2:G18" totalsRowShown="0">
+  <autoFilter ref="A2:G18">
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
+    <filterColumn colId="6"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="7">
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="0">
-      <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+E2</calculatedColumnFormula>
+    <tableColumn id="4" name="Plan suma" dataDxfId="11">
+      <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Rzecz suma"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="10"/>
+    <tableColumn id="7" name="Plan"/>
+    <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1921,11 +2844,11 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1934,12 +2857,12 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="125" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="123" customWidth="1"/>
-    <col min="10" max="10" width="11" style="121" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="120" customWidth="1"/>
+    <col min="10" max="10" width="11" style="118" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" customWidth="1"/>
@@ -1960,7 +2883,7 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="125" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
@@ -1972,36 +2895,36 @@
       <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="123" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="121" t="s">
+      <c r="I1" s="120" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="118" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="117">
+      <c r="E2" s="126">
         <v>2252</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="124">
+      <c r="I2" s="121">
         <v>41015</v>
       </c>
-      <c r="J2" s="121" t="s">
+      <c r="J2" s="118" t="s">
         <v>84</v>
       </c>
       <c r="L2" s="45" t="s">
@@ -2013,382 +2936,384 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="117">
+      <c r="E3" s="126">
         <v>650</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="124">
+      <c r="I3" s="121">
         <v>41100</v>
       </c>
-      <c r="J3" s="121" t="s">
+      <c r="J3" s="118" t="s">
         <v>84</v>
       </c>
       <c r="L3" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="119" t="s">
-        <v>141</v>
+      <c r="M3" s="116" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="117">
+      <c r="E4" s="126">
         <v>2800</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="124">
+      <c r="I4" s="121">
         <v>41197</v>
       </c>
-      <c r="J4" s="121" t="s">
+      <c r="J4" s="118" t="s">
         <v>84</v>
       </c>
       <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="119" t="s">
-        <v>142</v>
+      <c r="M4" s="116" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="117">
+        <v>121</v>
+      </c>
+      <c r="E5" s="126">
         <v>3000</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="124">
+      <c r="I5" s="121">
         <v>41351</v>
       </c>
-      <c r="J5" s="121" t="s">
+      <c r="J5" s="118" t="s">
         <v>84</v>
       </c>
       <c r="L5" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="120" t="s">
-        <v>143</v>
+      <c r="M5" s="117" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="117">
+      <c r="E6" s="126">
         <v>148</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="124">
+      <c r="I6" s="121">
         <v>41351</v>
       </c>
-      <c r="J6" s="121" t="s">
+      <c r="J6" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M6" s="120" t="s">
-        <v>144</v>
+      <c r="M6" s="117" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="114" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="114" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="117">
+      <c r="E7" s="126">
         <v>2142</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="124">
+      <c r="I7" s="121">
         <v>41352</v>
       </c>
-      <c r="J7" s="121" t="s">
+      <c r="J7" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M7" s="120" t="s">
-        <v>146</v>
+      <c r="M7" s="117" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="118">
+      <c r="E8" s="127">
         <v>400</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="124">
+      <c r="I8" s="121">
         <v>41353</v>
       </c>
-      <c r="J8" s="121" t="s">
+      <c r="J8" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M8" s="120" t="s">
-        <v>147</v>
+      <c r="M8" s="117" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" s="118">
+        <v>152</v>
+      </c>
+      <c r="E9" s="127">
         <v>260</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="124">
+      <c r="I9" s="121">
         <v>41360</v>
       </c>
-      <c r="J9" s="121" t="s">
+      <c r="J9" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M9" s="120" t="s">
-        <v>148</v>
+      <c r="M9" s="117" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="118">
+      <c r="E10" s="127">
         <v>600</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="124">
+      <c r="I10" s="121">
         <v>41362</v>
       </c>
-      <c r="J10" s="121" t="s">
+      <c r="J10" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M10" s="120" t="s">
-        <v>149</v>
+      <c r="M10" s="117" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="127">
         <v>416</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="124">
+      <c r="I11" s="121">
         <v>41367</v>
       </c>
-      <c r="J11" s="121" t="s">
+      <c r="J11" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M11" s="120" t="s">
-        <v>150</v>
+      <c r="M11" s="117" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="D12" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="117">
+      <c r="E12" s="126">
         <v>1000</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="124">
+      <c r="I12" s="121">
         <v>41372</v>
       </c>
-      <c r="J12" s="121" t="s">
+      <c r="J12" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M12" s="120" t="s">
-        <v>151</v>
+      <c r="M12" s="117" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" s="118">
+      <c r="E13" s="127">
         <v>1000</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="124">
+      <c r="I13" s="121">
         <v>41382</v>
       </c>
-      <c r="J13" s="121" t="s">
+      <c r="J13" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="M13" s="120" t="s">
-        <v>152</v>
+      <c r="M13" s="117" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="128">
         <v>150</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="124">
+      <c r="I14" s="121">
         <v>41391</v>
       </c>
-      <c r="J14" s="121" t="s">
+      <c r="J14" s="118" t="s">
         <v>84</v>
       </c>
       <c r="M14" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="128">
         <v>200</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="124">
+      <c r="I15" s="121">
         <v>41404</v>
       </c>
-      <c r="J15" s="121" t="s">
+      <c r="J15" s="118" t="s">
         <v>84</v>
       </c>
       <c r="M15" s="111" t="s">
@@ -2397,27 +3322,27 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D16" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="128">
         <v>140</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="124">
+      <c r="I16" s="121">
         <v>41406</v>
       </c>
-      <c r="J16" s="121" t="s">
+      <c r="J16" s="118" t="s">
         <v>84</v>
       </c>
       <c r="M16" s="111" t="s">
@@ -2426,143 +3351,143 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="128">
         <v>200</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="124">
+      <c r="I17" s="121">
         <v>41428</v>
       </c>
-      <c r="J17" s="121" t="s">
+      <c r="J17" s="118" t="s">
         <v>84</v>
       </c>
       <c r="M17" s="111" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="128">
         <v>200</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="124">
+      <c r="I18" s="121">
         <v>41484</v>
       </c>
-      <c r="J18" s="121" t="s">
+      <c r="J18" s="118" t="s">
         <v>84</v>
       </c>
       <c r="M18" s="111" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="10">
+      <c r="E19" s="128">
         <v>147</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="124">
+      <c r="I19" s="121">
         <v>41488</v>
       </c>
-      <c r="J19" s="121" t="s">
+      <c r="J19" s="118" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" s="116">
+      <c r="E20" s="129">
         <v>450</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="124">
+      <c r="I20" s="121">
         <v>41515</v>
       </c>
-      <c r="J20" s="121" t="s">
+      <c r="J20" s="118" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E21" s="116">
+        <v>139</v>
+      </c>
+      <c r="E21" s="129">
         <v>260</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="124">
+      <c r="I21" s="121">
         <v>41509</v>
       </c>
-      <c r="J21" s="121" t="s">
+      <c r="J21" s="118" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22" s="44" t="s">
         <v>86</v>
@@ -2573,7 +3498,7 @@
       <c r="D22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="130">
         <v>1510.21</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -2585,7 +3510,7 @@
       <c r="H22" s="3">
         <v>41497</v>
       </c>
-      <c r="I22" s="125">
+      <c r="I22" s="122">
         <v>41495</v>
       </c>
       <c r="J22" s="4" t="s">
@@ -2594,7 +3519,7 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23" s="44" t="s">
         <v>86</v>
@@ -2605,7 +3530,7 @@
       <c r="D23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="130">
         <v>5878.78</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -2617,7 +3542,7 @@
       <c r="H23" s="3">
         <v>41501</v>
       </c>
-      <c r="I23" s="125">
+      <c r="I23" s="122">
         <v>41501</v>
       </c>
       <c r="J23" s="4" t="s">
@@ -2626,7 +3551,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B24" s="44" t="s">
         <v>86</v>
@@ -2637,7 +3562,7 @@
       <c r="D24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="130">
         <v>19.079999999999998</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -2649,7 +3574,7 @@
       <c r="H24" s="3">
         <v>41501</v>
       </c>
-      <c r="I24" s="125">
+      <c r="I24" s="122">
         <v>41501</v>
       </c>
       <c r="J24" s="4" t="s">
@@ -2658,7 +3583,7 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B25" s="44" t="s">
         <v>86</v>
@@ -2669,7 +3594,7 @@
       <c r="D25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="130">
         <v>115.01</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -2681,7 +3606,7 @@
       <c r="H25" s="3">
         <v>41501</v>
       </c>
-      <c r="I25" s="125">
+      <c r="I25" s="122">
         <v>41501</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -2690,7 +3615,7 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B26" s="44" t="s">
         <v>86</v>
@@ -2701,7 +3626,7 @@
       <c r="D26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="130">
         <v>8280.36</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -2713,7 +3638,7 @@
       <c r="H26" s="3">
         <v>41502</v>
       </c>
-      <c r="I26" s="125">
+      <c r="I26" s="122">
         <v>41501</v>
       </c>
       <c r="J26" s="4" t="s">
@@ -2722,7 +3647,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>86</v>
@@ -2733,7 +3658,7 @@
       <c r="D27" t="s">
         <v>17</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="125">
         <v>1657.43</v>
       </c>
       <c r="F27" t="s">
@@ -2745,16 +3670,16 @@
       <c r="H27" s="2">
         <v>41505</v>
       </c>
-      <c r="I27" s="125">
+      <c r="I27" s="122">
         <v>41502</v>
       </c>
-      <c r="J27" s="121" t="s">
+      <c r="J27" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B28" s="44" t="s">
         <v>86</v>
@@ -2765,7 +3690,7 @@
       <c r="D28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="130">
         <v>512.29999999999995</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -2777,87 +3702,90 @@
       <c r="H28" s="3">
         <v>41509</v>
       </c>
-      <c r="I28" s="125">
+      <c r="I28" s="122">
         <v>41507</v>
       </c>
-      <c r="J28" s="121" t="s">
+      <c r="J28" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B29" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>35</v>
+      <c r="C29" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="125">
         <v>10584</v>
       </c>
-      <c r="I29" s="125">
+      <c r="F29" t="s">
+        <v>157</v>
+      </c>
+      <c r="I29" s="122">
         <v>41507</v>
       </c>
-      <c r="J29" s="121" t="s">
+      <c r="J29" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B30" s="44" t="s">
         <v>87</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
         <v>78</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="125">
         <v>400</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="125">
+      <c r="I30" s="122">
         <v>41474</v>
       </c>
-      <c r="J30" s="121" t="s">
+      <c r="J30" s="118" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B31" s="44" t="s">
         <v>87</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
         <v>79</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="125">
         <v>650</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="125">
+      <c r="I31" s="122">
         <v>41474</v>
       </c>
-      <c r="J31" s="121" t="s">
+      <c r="J31" s="118" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B32" s="44" t="s">
         <v>86</v>
@@ -2868,38 +3796,47 @@
       <c r="D32" t="s">
         <v>8</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="125">
         <v>7800</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="125">
+      <c r="I32" s="122">
         <v>41474</v>
       </c>
-      <c r="J32" s="121" t="s">
+      <c r="J32" s="118" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B33" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="C33" t="s">
-        <v>35</v>
+      <c r="C33" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="D33" t="s">
         <v>34</v>
       </c>
-      <c r="E33">
-        <v>335</v>
+      <c r="E33" s="125">
+        <v>335.18</v>
+      </c>
+      <c r="F33" t="s">
+        <v>154</v>
       </c>
       <c r="H33" s="1"/>
+      <c r="I33" s="122">
+        <v>41521</v>
+      </c>
+      <c r="J33" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B34" s="44" t="s">
         <v>86</v>
@@ -2910,11 +3847,11 @@
       <c r="D34" t="s">
         <v>80</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="125">
         <v>7610.63</v>
       </c>
       <c r="F34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G34" s="2">
         <v>41514</v>
@@ -2922,16 +3859,16 @@
       <c r="H34" s="112">
         <v>41517</v>
       </c>
-      <c r="I34" s="125">
+      <c r="I34" s="122">
         <v>41515</v>
       </c>
-      <c r="J34" s="121" t="s">
+      <c r="J34" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B35" s="44" t="s">
         <v>86</v>
@@ -2940,13 +3877,13 @@
         <v>89</v>
       </c>
       <c r="D35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="125">
+        <v>992.96</v>
+      </c>
+      <c r="F35" t="s">
         <v>114</v>
-      </c>
-      <c r="E35">
-        <v>992.96</v>
-      </c>
-      <c r="F35" t="s">
-        <v>115</v>
       </c>
       <c r="G35" s="2">
         <v>41492</v>
@@ -2954,67 +3891,76 @@
       <c r="H35" s="2">
         <v>41495</v>
       </c>
-      <c r="I35" s="125">
+      <c r="I35" s="122">
         <v>41516</v>
       </c>
-      <c r="J35" s="121" t="s">
+      <c r="J35" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B36" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>35</v>
+      <c r="C36" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="D36" t="s">
         <v>28</v>
       </c>
-      <c r="E36">
-        <v>7236</v>
+      <c r="E36" s="125">
+        <v>7010.82</v>
+      </c>
+      <c r="F36" t="s">
+        <v>153</v>
+      </c>
+      <c r="I36" s="122">
+        <v>41521</v>
+      </c>
+      <c r="J36" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>35</v>
+      <c r="C37" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="D37" t="s">
         <v>30</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="125">
         <v>3078</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B38" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>35</v>
+      <c r="C38" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="D38" t="s">
         <v>31</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="125">
         <v>2052</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B39" s="44" t="s">
         <v>86</v>
@@ -3023,13 +3969,13 @@
         <v>89</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="128">
+        <v>3813.05</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="E39" s="1">
-        <v>3813.05</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="G39" s="112">
         <v>41512</v>
@@ -3037,16 +3983,16 @@
       <c r="H39" s="112">
         <v>41519</v>
       </c>
-      <c r="I39" s="125">
+      <c r="I39" s="122">
         <v>41515</v>
       </c>
-      <c r="J39" s="121" t="s">
+      <c r="J39" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="44" t="s">
         <v>86</v>
@@ -3055,13 +4001,13 @@
         <v>89</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="128">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E40" s="1">
-        <v>66.180000000000007</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="G40" s="112">
         <v>41513</v>
@@ -3069,16 +4015,16 @@
       <c r="H40" s="112">
         <v>41516</v>
       </c>
-      <c r="I40" s="125">
+      <c r="I40" s="122">
         <v>41515</v>
       </c>
-      <c r="J40" s="121" t="s">
+      <c r="J40" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B41" s="44" t="s">
         <v>86</v>
@@ -3087,13 +4033,13 @@
         <v>89</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="128">
+        <v>649.32000000000005</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E41" s="1">
-        <v>649.32000000000005</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G41" s="112">
         <v>41513</v>
@@ -3101,16 +4047,16 @@
       <c r="H41" s="112">
         <v>41516</v>
       </c>
-      <c r="I41" s="125">
+      <c r="I41" s="122">
         <v>41515</v>
       </c>
-      <c r="J41" s="121" t="s">
+      <c r="J41" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B42" s="44" t="s">
         <v>86</v>
@@ -3119,133 +4065,196 @@
         <v>89</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="128">
+        <v>3084.07</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="E42" s="1">
-        <v>3084.07</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="G42" s="112">
         <v>41516</v>
       </c>
       <c r="H42" s="112">
-        <v>41307</v>
-      </c>
-      <c r="I42" s="124">
+        <v>41519</v>
+      </c>
+      <c r="I42" s="121">
         <v>41516</v>
       </c>
-      <c r="J42" s="121" t="s">
+      <c r="J42" s="118" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B43" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43">
-        <v>10584</v>
+        <v>86</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="128">
+        <v>54</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G43" s="112"/>
+      <c r="H43" s="112"/>
+      <c r="I43" s="121">
+        <v>41521</v>
+      </c>
+      <c r="J43" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="42" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44">
-        <v>5724</v>
+        <v>86</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="128">
+        <v>1415.36</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G44" s="112">
+        <v>41516</v>
+      </c>
+      <c r="H44" s="112">
+        <v>41519</v>
+      </c>
+      <c r="I44" s="121">
+        <v>41521</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B45" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>35</v>
+      <c r="C45" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="D45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="125">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="125">
+        <v>5724</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" t="s">
         <v>33</v>
       </c>
-      <c r="E45">
+      <c r="E47" s="125">
         <v>6372</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A53" s="47" t="s">
+    <row r="55" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A55" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="47"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47">
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="131">
         <f>SUBTOTAL(109,[Kwota])</f>
-        <v>105419.38</v>
-      </c>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="126"/>
-      <c r="J53" s="122">
+        <v>106663.74</v>
+      </c>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="123"/>
+      <c r="J55" s="119">
         <f>SUBTOTAL(103,[Konto])</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" thickTop="1"/>
-    <row r="61" spans="1:10">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="127"/>
-      <c r="J61" s="115"/>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="127"/>
-      <c r="J78" s="115"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="63" spans="1:10">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="128"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="124"/>
+      <c r="J63" s="115"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="D65">
+        <f>7400-54-335.18</f>
+        <v>7010.82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="128"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="124"/>
+      <c r="J80" s="115"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A54:A61">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A56:A63">
       <formula1>$M$4:$M$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B61 B50:B52 B22:B45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56:B63 B52:B54 B22:B47">
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A54">
       <formula1>$M$3:$M$18</formula1>
     </dataValidation>
   </dataValidations>
@@ -3260,250 +4269,449 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F18"/>
+  <dimension ref="A3:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="3" spans="1:2">
+      <c r="A3" s="132" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="46">
+        <v>16415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="134" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="46">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="134" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="46">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="134" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="46">
+        <v>5197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="134" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="46">
+        <v>8492</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="133" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="46">
+        <v>46345.939999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="134" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="46">
+        <v>34711.939999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="134" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="46">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="134" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="46">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="133" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="46">
+        <v>21222.800000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="134" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="46">
+        <v>9081.9800000000014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="134" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="46">
+        <v>12140.82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="133" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="46">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="134" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="46">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="133" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="46">
+        <v>12096</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="134" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="46">
+        <v>12096</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="133" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="46"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="134" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" s="46"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="133" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="46">
+        <v>106663.73999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="110"/>
       <c r="B1" s="110"/>
       <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-    </row>
-    <row r="2" spans="2:6">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>94</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="46">
         <v>0</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>43</v>
       </c>
+      <c r="B4">
+        <v>37600</v>
+      </c>
       <c r="C4">
+        <v>46700</v>
+      </c>
+      <c r="D4" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D3</f>
         <v>37600</v>
       </c>
-      <c r="D4">
-        <v>46700</v>
-      </c>
       <c r="E4" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E3</f>
-        <v>37600</v>
-      </c>
-      <c r="F4" s="46">
         <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
         <v>9100</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" t="s">
+      <c r="F4" s="2">
+        <v>41499</v>
+      </c>
+      <c r="G4" s="2">
+        <v>41499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="C5">
+      <c r="B5">
         <v>37800</v>
       </c>
-      <c r="E5" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E4</f>
+      <c r="D5" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D4</f>
         <v>75400</v>
       </c>
-      <c r="F5" s="46"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" t="s">
+      <c r="E5" s="46"/>
+      <c r="F5" s="2">
+        <v>41544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>43200</v>
+      </c>
+      <c r="D6" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D5</f>
+        <v>118600</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="2">
+        <v>41536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>47500</v>
+      </c>
+      <c r="D7" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D6</f>
+        <v>166100</v>
+      </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="2">
+        <v>41571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <v>32000</v>
+      </c>
+      <c r="D8" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D7</f>
+        <v>198100</v>
+      </c>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>21600</v>
+      </c>
+      <c r="D9" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D8</f>
+        <v>219700</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>9700</v>
+      </c>
+      <c r="D10" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D9</f>
+        <v>229400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>45700</v>
+      </c>
+      <c r="D11" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D10</f>
+        <v>275100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>16200</v>
+      </c>
+      <c r="D12" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D11</f>
+        <v>291300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>22200</v>
+      </c>
+      <c r="D13" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D12</f>
+        <v>313500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>39900</v>
+      </c>
+      <c r="D14" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D13</f>
+        <v>353400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15">
+        <v>6500</v>
+      </c>
+      <c r="D15" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D14</f>
+        <v>359900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>31300</v>
+      </c>
+      <c r="D16" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D15</f>
+        <v>391200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>98</v>
       </c>
-      <c r="C6">
-        <v>43200</v>
-      </c>
-      <c r="E6" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E5</f>
-        <v>118600</v>
-      </c>
-      <c r="F6" s="46"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <v>47500</v>
-      </c>
-      <c r="E7" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E6</f>
-        <v>166100</v>
-      </c>
-      <c r="F7" s="46"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8">
-        <v>32000</v>
-      </c>
-      <c r="E8" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E7</f>
-        <v>198100</v>
-      </c>
-      <c r="F8" s="46"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9">
-        <v>21600</v>
-      </c>
-      <c r="E9" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E8</f>
-        <v>219700</v>
-      </c>
-      <c r="F9" s="46"/>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10">
-        <v>9700</v>
-      </c>
-      <c r="E10" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E9</f>
-        <v>229400</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11">
-        <v>45700</v>
-      </c>
-      <c r="E11" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E10</f>
-        <v>275100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12">
-        <v>16200</v>
-      </c>
-      <c r="E12" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E11</f>
-        <v>291300</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13">
-        <v>22200</v>
-      </c>
-      <c r="E13" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E12</f>
-        <v>313500</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14">
-        <v>39900</v>
-      </c>
-      <c r="E14" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E13</f>
-        <v>353400</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15">
-        <v>6500</v>
-      </c>
-      <c r="E15" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E14</f>
-        <v>359900</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16">
-        <v>31300</v>
-      </c>
-      <c r="E16" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E15</f>
-        <v>391200</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
+      <c r="B17">
+        <v>20000</v>
+      </c>
+      <c r="D17" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D16</f>
+        <v>411200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>99</v>
       </c>
-      <c r="C17">
-        <v>20000</v>
-      </c>
-      <c r="E17" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E16</f>
-        <v>411200</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18">
+      <c r="B18">
         <v>31600</v>
       </c>
-      <c r="E18" s="46">
-        <f>Tabela5[[#This Row],[Planowane]]+E17</f>
+      <c r="D18" s="46">
+        <f>Tabela5[[#This Row],[Planowane]]+D17</f>
         <v>442800</v>
       </c>
     </row>
@@ -3516,12 +4724,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3552,7 +4760,7 @@
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -3632,7 +4840,7 @@
       </c>
       <c r="G4" s="19"/>
       <c r="J4" s="97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K4" s="97">
         <v>43200</v>
@@ -3684,7 +4892,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
       <c r="J6" s="99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K6" s="99">
         <v>32000</v>
@@ -3822,7 +5030,7 @@
       <c r="F11" s="40"/>
       <c r="G11" s="41"/>
       <c r="J11" s="104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="104">
         <v>22200</v>
@@ -3849,7 +5057,7 @@
       <c r="F12" s="40"/>
       <c r="G12" s="41"/>
       <c r="J12" s="105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K12" s="105">
         <v>39900</v>
@@ -3930,7 +5138,7 @@
       <c r="F15" s="88"/>
       <c r="G15" s="89"/>
       <c r="J15" s="108" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K15" s="108">
         <v>20000</v>
@@ -3957,7 +5165,7 @@
       <c r="F16" s="83"/>
       <c r="G16" s="84"/>
       <c r="J16" s="108" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K16" s="108">
         <v>31600</v>

</xml_diff>

<commit_message>
lepsza tabelka - filtr
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" showPivotChartFilter="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" hidePivotFieldList="1" showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="13020" windowHeight="2895" activeTab="1"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="169">
   <si>
     <t>Opis</t>
   </si>
@@ -555,9 +555,6 @@
   </si>
   <si>
     <t>Etykiety wierszy</t>
-  </si>
-  <si>
-    <t>(puste)</t>
   </si>
   <si>
     <t>Suma końcowa</t>
@@ -1039,7 +1036,27 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="3"/>
@@ -2371,7 +2388,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:H11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
@@ -2386,12 +2403,12 @@
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
       <items count="7">
-        <item x="2"/>
+        <item h="1" x="2"/>
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item x="4"/>
-        <item sd="0" x="5"/>
+        <item h="1" sd="0" x="5"/>
         <item t="default" sd="0"/>
       </items>
     </pivotField>
@@ -2407,7 +2424,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -2423,9 +2440,6 @@
     <i>
       <x v="4"/>
     </i>
-    <i>
-      <x v="5"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -2433,10 +2447,7 @@
   <colFields count="1">
     <field x="1"/>
   </colFields>
-  <colItems count="7">
-    <i>
-      <x/>
-    </i>
+  <colItems count="5">
     <i>
       <x v="1"/>
     </i>
@@ -2449,9 +2460,6 @@
     <i>
       <x v="4"/>
     </i>
-    <i>
-      <x v="5"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -2460,14 +2468,14 @@
     <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="5">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="4">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2489,16 +2497,16 @@
     <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="16"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="15"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="14"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="13"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="10"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="9"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="8"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="20"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="19"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="17"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="14"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="13"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="12"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2516,10 +2524,10 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="3">
+    <tableColumn id="4" name="Plan suma" dataDxfId="7">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Rzecz różnica" dataDxfId="2"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="6"/>
     <tableColumn id="7" name="Plan"/>
     <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
@@ -3183,7 +3191,7 @@
         <v>128</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" s="115" t="s">
         <v>4</v>
@@ -4240,21 +4248,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:H11"/>
+  <dimension ref="A3:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
     <col min="10" max="10" width="7.140625" customWidth="1"/>
@@ -4278,166 +4285,132 @@
     <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:6">
       <c r="A3" s="132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="132" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="132" t="s">
         <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
         <v>165</v>
       </c>
-      <c r="H4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="133" t="s">
         <v>140</v>
       </c>
       <c r="B5" s="46">
-        <v>2526</v>
+        <v>200</v>
       </c>
       <c r="C5" s="46">
-        <v>200</v>
+        <v>5197</v>
       </c>
       <c r="D5" s="46">
-        <v>5197</v>
-      </c>
-      <c r="E5" s="46">
         <v>8492</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="134">
-        <v>16415</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="E5" s="46"/>
+      <c r="F5" s="134">
+        <v>13889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="133" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46">
+      <c r="B6" s="46">
         <v>34711.939999999995</v>
       </c>
-      <c r="D6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46">
+        <v>1050</v>
+      </c>
       <c r="E6" s="46">
-        <v>1050</v>
-      </c>
-      <c r="F6" s="46">
         <v>10584</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="134">
+      <c r="F6" s="134">
         <v>46345.939999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:6">
       <c r="A7" s="133" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46">
-        <v>9081.9800000000014</v>
-      </c>
+      <c r="B7" s="46">
+        <v>9081.98</v>
+      </c>
+      <c r="C7" s="46"/>
       <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46">
+      <c r="E7" s="46">
         <v>12140.82</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="H7" s="134">
-        <v>21222.800000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="F7" s="134">
+        <v>21222.799999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="133" t="s">
         <v>143</v>
       </c>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
       <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46">
+      <c r="E8" s="46">
         <v>10584</v>
       </c>
-      <c r="G8" s="46"/>
-      <c r="H8" s="134">
+      <c r="F8" s="134">
         <v>10584</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:6">
       <c r="A9" s="133" t="s">
         <v>145</v>
       </c>
       <c r="B9" s="46"/>
       <c r="C9" s="46"/>
       <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46">
+      <c r="E9" s="46">
         <v>12096</v>
       </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="134">
+      <c r="F9" s="134">
         <v>12096</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:6">
       <c r="A10" s="133" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="134"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="133" t="s">
-        <v>166</v>
-      </c>
-      <c r="B11" s="46">
-        <v>2526</v>
-      </c>
-      <c r="C11" s="46">
+      <c r="B10" s="46">
         <v>43993.919999999998</v>
       </c>
-      <c r="D11" s="46">
+      <c r="C10" s="46">
         <v>5197</v>
       </c>
-      <c r="E11" s="46">
+      <c r="D10" s="46">
         <v>9542</v>
       </c>
-      <c r="F11" s="46">
+      <c r="E10" s="46">
         <v>45404.82</v>
       </c>
-      <c r="G11" s="46"/>
-      <c r="H11" s="135">
-        <v>106663.73999999999</v>
+      <c r="F10" s="135">
+        <v>104137.73999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lepsza tabelka - sortowanie po koszcie
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -18,7 +18,7 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="33" r:id="rId5"/>
+    <pivotCache cacheId="34" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="169">
   <si>
     <t>Opis</t>
   </si>
@@ -1036,7 +1036,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="25">
     <dxf>
       <font>
         <b/>
@@ -1059,6 +1059,11 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="3"/>
       </font>
     </dxf>
@@ -1068,10 +1073,25 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1610,25 +1630,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="46088576"/>
-        <c:axId val="46091264"/>
+        <c:axId val="44841600"/>
+        <c:axId val="46090112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46088576"/>
+        <c:axId val="44841600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46091264"/>
+        <c:crossAx val="46090112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46091264"/>
+        <c:axId val="46090112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1657,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46088576"/>
+        <c:crossAx val="44841600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1650,7 +1670,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2387,8 +2407,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
@@ -2401,9 +2421,9 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="descending">
       <items count="7">
-        <item h="1" x="2"/>
+        <item x="2"/>
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
@@ -2411,6 +2431,15 @@
         <item h="1" sd="0" x="5"/>
         <item t="default" sd="0"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2447,18 +2476,21 @@
   <colFields count="1">
     <field x="1"/>
   </colFields>
-  <colItems count="5">
+  <colItems count="6">
+    <i>
+      <x v="4"/>
+    </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
+      <x/>
     </i>
     <i t="grand">
       <x/>
@@ -2468,14 +2500,14 @@
     <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="11">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="10">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2497,16 +2529,16 @@
     <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="20"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="19"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="17"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="14"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="13"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="12"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="24"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="23"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="22"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="21"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="18"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="17"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2524,10 +2556,10 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="7">
+    <tableColumn id="4" name="Plan suma" dataDxfId="9">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Rzecz różnica" dataDxfId="6"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="8"/>
     <tableColumn id="7" name="Plan"/>
     <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
@@ -4248,20 +4280,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:F10"/>
+  <dimension ref="A3:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
     <col min="10" max="10" width="7.140625" customWidth="1"/>
@@ -4285,7 +4318,7 @@
     <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="132" t="s">
         <v>166</v>
       </c>
@@ -4293,124 +4326,137 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="132" t="s">
         <v>164</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
       </c>
       <c r="D4" t="s">
         <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="133" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="46"/>
+      <c r="C5" s="46">
         <v>200</v>
-      </c>
-      <c r="C5" s="46">
-        <v>5197</v>
       </c>
       <c r="D5" s="46">
         <v>8492</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="134">
-        <v>13889</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="46">
+        <v>5197</v>
+      </c>
+      <c r="F5" s="46">
+        <v>2526</v>
+      </c>
+      <c r="G5" s="134">
+        <v>16415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="133" t="s">
         <v>141</v>
       </c>
       <c r="B6" s="46">
+        <v>10584</v>
+      </c>
+      <c r="C6" s="46">
         <v>34711.939999999995</v>
       </c>
-      <c r="C6" s="46"/>
       <c r="D6" s="46">
         <v>1050</v>
       </c>
-      <c r="E6" s="46">
-        <v>10584</v>
-      </c>
-      <c r="F6" s="134">
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="134">
         <v>46345.939999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="133" t="s">
         <v>142</v>
       </c>
       <c r="B7" s="46">
-        <v>9081.98</v>
-      </c>
-      <c r="C7" s="46"/>
+        <v>12140.82</v>
+      </c>
+      <c r="C7" s="46">
+        <v>9081.9800000000014</v>
+      </c>
       <c r="D7" s="46"/>
-      <c r="E7" s="46">
-        <v>12140.82</v>
-      </c>
-      <c r="F7" s="134">
-        <v>21222.799999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="134">
+        <v>21222.800000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="133" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="46"/>
+      <c r="B8" s="46">
+        <v>10584</v>
+      </c>
       <c r="C8" s="46"/>
       <c r="D8" s="46"/>
-      <c r="E8" s="46">
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="134">
         <v>10584</v>
       </c>
-      <c r="F8" s="134">
-        <v>10584</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="133" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="46"/>
+      <c r="B9" s="46">
+        <v>12096</v>
+      </c>
       <c r="C9" s="46"/>
       <c r="D9" s="46"/>
-      <c r="E9" s="46">
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="134">
         <v>12096</v>
       </c>
-      <c r="F9" s="134">
-        <v>12096</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="133" t="s">
         <v>165</v>
       </c>
       <c r="B10" s="46">
+        <v>45404.82</v>
+      </c>
+      <c r="C10" s="46">
         <v>43993.919999999998</v>
-      </c>
-      <c r="C10" s="46">
-        <v>5197</v>
       </c>
       <c r="D10" s="46">
         <v>9542</v>
       </c>
       <c r="E10" s="46">
-        <v>45404.82</v>
-      </c>
-      <c r="F10" s="135">
-        <v>104137.73999999999</v>
+        <v>5197</v>
+      </c>
+      <c r="F10" s="46">
+        <v>2526</v>
+      </c>
+      <c r="G10" s="135">
+        <v>106663.73999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kolejna stal na strop
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="175">
   <si>
     <t>Opis</t>
   </si>
@@ -582,6 +582,9 @@
   </si>
   <si>
     <t>5732/T/09/2013</t>
+  </si>
+  <si>
+    <t>5801/T/09/2013</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1652,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2495,8 +2498,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J60" totalsRowCount="1">
-  <autoFilter ref="A1:J59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J62" totalsRowCount="1">
+  <autoFilter ref="A1:J61">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
     <filterColumn colId="2">
@@ -2838,11 +2841,11 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4295,82 +4298,123 @@
       </c>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="44"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="1"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="122"/>
+      <c r="A58" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="125">
+        <v>227.55</v>
+      </c>
+      <c r="F58" t="s">
+        <v>174</v>
+      </c>
+      <c r="G58" s="2">
+        <v>41528</v>
+      </c>
+      <c r="H58" s="2">
+        <v>41531</v>
+      </c>
+      <c r="I58" s="122">
+        <v>41528</v>
+      </c>
+      <c r="J58" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="44"/>
       <c r="B59" s="44"/>
-      <c r="C59" s="1"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="122"/>
     </row>
-    <row r="60" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A60" s="47" t="s">
+    <row r="60" spans="1:10">
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="1"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="122"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="1"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="122"/>
+    </row>
+    <row r="62" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A62" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="131">
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="131">
         <f>SUBTOTAL(109,[Kwota])</f>
-        <v>43395.24</v>
-      </c>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="123"/>
-      <c r="J60" s="119">
+        <v>43622.79</v>
+      </c>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="123"/>
+      <c r="J62" s="119">
         <f>SUBTOTAL(103,[Konto])</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" thickTop="1"/>
-    <row r="68" spans="1:10">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="128"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="124"/>
-      <c r="J68" s="115"/>
-    </row>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" thickTop="1"/>
     <row r="70" spans="1:10">
-      <c r="D70">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="128"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="124"/>
+      <c r="J70" s="115"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="D72">
         <f>7400-54-335.18</f>
         <v>7010.82</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="128"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="124"/>
-      <c r="J85" s="115"/>
+    <row r="87" spans="1:10">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="128"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="124"/>
+      <c r="J87" s="115"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A61:A68">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A63:A70">
       <formula1>$M$4:$M$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61:B68 B22:B47 B52:B57">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63:B70 B22:B47 B52:B59">
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A61">
       <formula1>$M$3:$M$18</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Manex zwrócił za dwukrotnie zaplacona fakturę
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -23,42 +23,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="E28" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-dwa razy</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="175">
   <si>
@@ -594,7 +558,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -642,21 +606,6 @@
       <sz val="13"/>
       <color theme="3"/>
       <name val="Czcionka tekstu podstawowego"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1031,14 +980,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1049,13 +998,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1089,6 +1054,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1117,6 +1087,17 @@
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFC00000"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1244,6 +1225,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1366,41 +1350,6 @@
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1612,25 +1561,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62732544"/>
-        <c:axId val="62754816"/>
+        <c:axId val="63465728"/>
+        <c:axId val="63483904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62732544"/>
+        <c:axId val="63465728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62754816"/>
+        <c:crossAx val="63483904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62754816"/>
+        <c:axId val="63483904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1639,7 +1588,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62732544"/>
+        <c:crossAx val="63465728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1652,7 +1601,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2482,14 +2431,14 @@
     <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="13">
+    <format dxfId="3">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="2">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2515,16 +2464,16 @@
     <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="9"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="8"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="7"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="4"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="3"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="15" totalsRowDxfId="1"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="0"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="16"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="15"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="14"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="13"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="10"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="9"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="8"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2542,10 +2491,10 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="11">
+    <tableColumn id="4" name="Plan suma" dataDxfId="1">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Rzecz różnica" dataDxfId="10"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="0"/>
     <tableColumn id="7" name="Plan"/>
     <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
@@ -2845,7 +2794,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4420,9 +4369,8 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
stal strop i beton słupki
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -18,13 +18,13 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="177">
   <si>
     <t>Opis</t>
   </si>
@@ -549,6 +549,12 @@
   </si>
   <si>
     <t>5801/T/09/2013</t>
+  </si>
+  <si>
+    <t>5924/T/09/2013</t>
+  </si>
+  <si>
+    <t>Beton na słupki</t>
   </si>
 </sst>
 </file>
@@ -989,17 +995,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -1312,22 +1308,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
       </font>
@@ -1345,6 +1325,22 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1377,7 +1373,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1557,25 +1552,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63117568"/>
-        <c:axId val="63135744"/>
+        <c:axId val="62724352"/>
+        <c:axId val="62742528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63117568"/>
+        <c:axId val="62724352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63135744"/>
+        <c:crossAx val="62742528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63135744"/>
+        <c:axId val="62742528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,21 +1579,20 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63117568"/>
+        <c:crossAx val="62724352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2419,7 +2413,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -2512,14 +2506,14 @@
     <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="15">
+    <format dxfId="16">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="15">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2528,33 +2522,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J62" totalsRowCount="1">
-  <autoFilter ref="A1:J61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J59" totalsRowCount="1">
+  <autoFilter ref="A1:J58">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
     <filterColumn colId="3"/>
     <filterColumn colId="7"/>
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
+    <filterColumn colId="8"/>
   </autoFilter>
   <sortState ref="A2:J52">
     <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="11"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="10"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="9"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="7"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="6"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="5"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="17" totalsRowDxfId="3"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="9"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="8"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="7"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="4"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="3"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="11" totalsRowDxfId="1"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="10" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2572,10 +2562,10 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="13">
+    <tableColumn id="4" name="Plan suma" dataDxfId="14">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Rzecz różnica" dataDxfId="12"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="13"/>
     <tableColumn id="7" name="Plan"/>
     <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
@@ -2871,11 +2861,11 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3962,7 +3952,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>142</v>
       </c>
@@ -3983,7 +3973,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="118"/>
     </row>
-    <row r="38" spans="1:10" hidden="1">
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
         <v>142</v>
       </c>
@@ -4192,7 +4182,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>143</v>
       </c>
@@ -4213,7 +4203,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="118"/>
     </row>
-    <row r="46" spans="1:10" hidden="1">
+    <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
         <v>145</v>
       </c>
@@ -4234,7 +4224,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="118"/>
     </row>
-    <row r="47" spans="1:10" hidden="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
         <v>145</v>
       </c>
@@ -4255,291 +4245,283 @@
       <c r="H47" s="1"/>
       <c r="I47" s="118"/>
     </row>
-    <row r="48" spans="1:10" hidden="1">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="126"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="118"/>
-    </row>
-    <row r="49" spans="1:10" hidden="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="126"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="118"/>
-    </row>
-    <row r="50" spans="1:10" hidden="1">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="126"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="118"/>
-    </row>
-    <row r="51" spans="1:10" hidden="1">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="126"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="118"/>
-    </row>
-    <row r="52" spans="1:10" hidden="1">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="126"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="118"/>
-    </row>
-    <row r="53" spans="1:10" hidden="1">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="126"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="118"/>
-    </row>
-    <row r="54" spans="1:10" hidden="1">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E48" s="126">
+        <v>4163.04</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G48" s="1">
+        <v>41515</v>
+      </c>
+      <c r="H48" s="1">
+        <v>41518</v>
+      </c>
+      <c r="I48" s="118">
+        <v>41527</v>
+      </c>
+      <c r="J48" s="115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E49" s="126">
+        <v>1214.22</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G49" s="1">
+        <v>41515</v>
+      </c>
+      <c r="H49" s="1">
+        <v>41518</v>
+      </c>
+      <c r="I49" s="118">
+        <v>41527</v>
+      </c>
+      <c r="J49" s="115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="126">
+        <v>2413.2399999999998</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G50" s="1">
+        <v>41527</v>
+      </c>
+      <c r="H50" s="1">
+        <v>41530</v>
+      </c>
+      <c r="I50" s="118">
+        <v>41527</v>
+      </c>
+      <c r="J50" s="115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="126">
+        <v>227.55</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G51" s="1">
+        <v>41528</v>
+      </c>
+      <c r="H51" s="1">
+        <v>41531</v>
+      </c>
+      <c r="I51" s="118">
+        <v>41528</v>
+      </c>
+      <c r="J51" s="115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="122">
+        <v>247.93</v>
+      </c>
+      <c r="F52" t="s">
+        <v>175</v>
+      </c>
+      <c r="G52" s="2">
+        <v>41534</v>
+      </c>
+      <c r="H52" s="2">
+        <v>41537</v>
+      </c>
+      <c r="I52" s="119">
+        <v>41534</v>
+      </c>
+      <c r="J52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" s="122">
+        <v>360</v>
+      </c>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2">
+        <v>41537</v>
+      </c>
+      <c r="I53" s="119"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="42"/>
+      <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="126"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="118"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="119"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E55" s="126">
-        <v>4163.04</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G55" s="1">
-        <v>41515</v>
-      </c>
-      <c r="H55" s="1">
-        <v>41518</v>
-      </c>
-      <c r="I55" s="118">
-        <v>41527</v>
-      </c>
-      <c r="J55" s="115" t="s">
-        <v>23</v>
-      </c>
+      <c r="A55" s="42"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="1"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="119"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E56" s="126">
-        <v>1214.22</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G56" s="1">
-        <v>41515</v>
-      </c>
-      <c r="H56" s="1">
-        <v>41518</v>
-      </c>
-      <c r="I56" s="118">
-        <v>41527</v>
-      </c>
-      <c r="J56" s="115" t="s">
-        <v>23</v>
-      </c>
+      <c r="A56" s="42"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="1"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="119"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="126">
-        <v>2413.2399999999998</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G57" s="1">
-        <v>41527</v>
-      </c>
-      <c r="H57" s="1">
-        <v>41530</v>
-      </c>
-      <c r="I57" s="118">
-        <v>41527</v>
-      </c>
-      <c r="J57" s="115" t="s">
-        <v>23</v>
-      </c>
+      <c r="A57" s="42"/>
+      <c r="B57" s="42"/>
+      <c r="C57" s="1"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="119"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E58" s="126">
-        <v>227.55</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G58" s="1">
-        <v>41528</v>
-      </c>
-      <c r="H58" s="1">
-        <v>41531</v>
-      </c>
-      <c r="I58" s="118">
-        <v>41528</v>
-      </c>
-      <c r="J58" s="115" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" hidden="1">
-      <c r="A59" s="42"/>
-      <c r="B59" s="42"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="3"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="119"/>
-    </row>
-    <row r="60" spans="1:10" hidden="1">
-      <c r="A60" s="42"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="1"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="119"/>
-    </row>
-    <row r="61" spans="1:10" hidden="1">
-      <c r="A61" s="42"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="1"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="119"/>
-    </row>
-    <row r="62" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A62" s="45" t="s">
+      <c r="A58" s="42"/>
+      <c r="B58" s="42"/>
+      <c r="C58" s="1"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="119"/>
+    </row>
+    <row r="59" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A59" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B62" s="45"/>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="127">
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="127">
         <f>SUBTOTAL(109,[Kwota])</f>
-        <v>86871.790000000008</v>
-      </c>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="45"/>
-      <c r="I62" s="120"/>
-      <c r="J62" s="116">
+        <v>115289.72</v>
+      </c>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="120"/>
+      <c r="J59" s="116">
         <f>SUBTOTAL(103,[Konto])</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" thickTop="1"/>
-    <row r="70" spans="1:10">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="125"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="121"/>
-      <c r="J70" s="112"/>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="125"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="121"/>
-      <c r="J87" s="112"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="67" spans="1:10">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="125"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="121"/>
+      <c r="J67" s="112"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="125"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="121"/>
+      <c r="J84" s="112"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A63:A70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60:A67">
       <formula1>$M$4:$M$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63:B70 B22:B47 B52:B59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B67 B22:B52">
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A61">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A58">
       <formula1>$M$3:$M$18</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
planowane do zapłaty za strop i schody
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -18,13 +18,13 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="178">
   <si>
     <t>Opis</t>
   </si>
@@ -533,9 +533,6 @@
     <t>Etykiety kolumn</t>
   </si>
   <si>
-    <t>o</t>
-  </si>
-  <si>
     <t>Bloczki</t>
   </si>
   <si>
@@ -560,7 +557,7 @@
     <t>5991/T/09/2013</t>
   </si>
   <si>
-    <t>2013-09-190</t>
+    <t>Belki, pustaki</t>
   </si>
 </sst>
 </file>
@@ -570,7 +567,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +646,14 @@
     <font>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -857,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -997,11 +1002,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1314,6 +1330,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1379,6 +1405,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1558,25 +1585,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71754880"/>
-        <c:axId val="71756416"/>
+        <c:axId val="66937984"/>
+        <c:axId val="71017600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71754880"/>
+        <c:axId val="66937984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71756416"/>
+        <c:crossAx val="71017600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71756416"/>
+        <c:axId val="71017600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1585,20 +1612,21 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71754880"/>
+        <c:crossAx val="66937984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1640,7 +1668,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="41532.416864467596" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="60">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="41538.576876388892" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="59">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabela1"/>
   </cacheSource>
@@ -1678,13 +1706,13 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Data faktury" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-08-06T00:00:00" maxDate="2013-09-12T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-08-06T00:00:00" maxDate="2013-09-20T00:00:00"/>
     </cacheField>
     <cacheField name="Data płatności" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-08-09T00:00:00" maxDate="2013-09-15T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-08-09T00:00:00" maxDate="2013-09-23T00:00:00"/>
     </cacheField>
-    <cacheField name="Zapłacono" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2012-04-16T00:00:00" maxDate="2013-09-12T00:00:00"/>
+    <cacheField name="Zapłacono" numFmtId="14">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2012-04-16T00:00:00" maxDate="2013-09-21T00:00:00"/>
     </cacheField>
     <cacheField name="Konto" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -1694,7 +1722,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="60">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="59">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -2224,6 +2252,30 @@
     <m/>
   </r>
   <r>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Manex"/>
+    <s v="Beton"/>
+    <n v="4489.5"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Manex"/>
+    <s v="Belki, pustaki"/>
+    <n v="7261.15"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <x v="4"/>
     <x v="4"/>
     <s v="Antoni Nowak"/>
@@ -2241,90 +2293,6 @@
     <s v="Antoni Nowak"/>
     <s v="Dach"/>
     <n v="6372"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
     <m/>
     <m/>
     <m/>
@@ -2356,7 +2324,7 @@
     <s v="eb wsp"/>
   </r>
   <r>
-    <x v="2"/>
+    <x v="3"/>
     <x v="3"/>
     <s v="Manex"/>
     <s v="Stal"/>
@@ -2380,6 +2348,54 @@
     <s v="eb wsp"/>
   </r>
   <r>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Manex"/>
+    <s v="Stal"/>
+    <n v="247.93"/>
+    <s v="5924/T/09/2013"/>
+    <d v="2013-09-17T00:00:00"/>
+    <d v="2013-09-20T00:00:00"/>
+    <d v="2013-09-17T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="Antoni Nowak"/>
+    <s v="Beton na słupki"/>
+    <n v="360"/>
+    <m/>
+    <m/>
+    <d v="2013-09-20T00:00:00"/>
+    <d v="2013-09-20T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Manex"/>
+    <s v="Stal"/>
+    <n v="257.38"/>
+    <s v="5991/T/09/2013"/>
+    <d v="2013-09-19T00:00:00"/>
+    <d v="2013-09-22T00:00:00"/>
+    <d v="2013-09-19T00:00:00"/>
+    <s v="eb wsp"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <x v="5"/>
     <x v="5"/>
     <m/>
@@ -2419,7 +2435,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -2512,14 +2528,14 @@
     <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="13">
+    <format dxfId="17">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="16">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2528,8 +2544,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J59" totalsRowCount="1">
-  <autoFilter ref="A1:J58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J61" totalsRowCount="1">
+  <autoFilter ref="A1:J60">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
@@ -2541,16 +2557,16 @@
     <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="9"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="8"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="7"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="4"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="3"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="15" totalsRowDxfId="1"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="0"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="11"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="10"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="9"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="7"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="6"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="5"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="19" totalsRowDxfId="3"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="18" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2568,10 +2584,10 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="11">
+    <tableColumn id="4" name="Plan suma" dataDxfId="15">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Rzecz różnica" dataDxfId="10"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="14"/>
     <tableColumn id="7" name="Plan"/>
     <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
@@ -2867,11 +2883,11 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3527,10 +3543,10 @@
       <c r="F22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
         <v>41494</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="2">
         <v>41497</v>
       </c>
       <c r="I22" s="118">
@@ -3559,10 +3575,10 @@
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2">
         <v>41494</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="2">
         <v>41501</v>
       </c>
       <c r="I23" s="118">
@@ -3591,10 +3607,10 @@
       <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="2">
         <v>41498</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="2">
         <v>41501</v>
       </c>
       <c r="I24" s="118">
@@ -3623,10 +3639,10 @@
       <c r="F25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="2">
         <v>41498</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="2">
         <v>41501</v>
       </c>
       <c r="I25" s="118">
@@ -3655,10 +3671,10 @@
       <c r="F26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="2">
         <v>41499</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="2">
         <v>41502</v>
       </c>
       <c r="I26" s="118">
@@ -3687,10 +3703,10 @@
       <c r="F27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2">
         <v>41502</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="2">
         <v>41505</v>
       </c>
       <c r="I27" s="118">
@@ -3719,10 +3735,10 @@
       <c r="F28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2">
         <v>41502</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="2">
         <v>41509</v>
       </c>
       <c r="I28" s="118">
@@ -3751,8 +3767,8 @@
       <c r="F29" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
       <c r="I29" s="118">
         <v>41507</v>
       </c>
@@ -3777,8 +3793,8 @@
         <v>400</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
       <c r="I30" s="118">
         <v>41474</v>
       </c>
@@ -3803,8 +3819,8 @@
         <v>650</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="118">
         <v>41474</v>
       </c>
@@ -3829,8 +3845,8 @@
         <v>7800</v>
       </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
       <c r="I32" s="118">
         <v>41474</v>
       </c>
@@ -3857,8 +3873,8 @@
       <c r="F33" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
       <c r="I33" s="118">
         <v>41521</v>
       </c>
@@ -3885,10 +3901,10 @@
       <c r="F34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="2">
         <v>41514</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="2">
         <v>41517</v>
       </c>
       <c r="I34" s="118">
@@ -3917,10 +3933,10 @@
       <c r="F35" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="2">
         <v>41492</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="2">
         <v>41495</v>
       </c>
       <c r="I35" s="118">
@@ -3949,8 +3965,8 @@
       <c r="F36" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
       <c r="I36" s="118">
         <v>41521</v>
       </c>
@@ -3975,8 +3991,8 @@
         <v>3078</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
       <c r="I37" s="118"/>
     </row>
     <row r="38" spans="1:10">
@@ -3996,8 +4012,8 @@
         <v>2052</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
       <c r="I38" s="118"/>
     </row>
     <row r="39" spans="1:10">
@@ -4019,10 +4035,10 @@
       <c r="F39" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="2">
         <v>41512</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="2">
         <v>41519</v>
       </c>
       <c r="I39" s="118">
@@ -4051,10 +4067,10 @@
       <c r="F40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="2">
         <v>41513</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="2">
         <v>41516</v>
       </c>
       <c r="I40" s="118">
@@ -4083,10 +4099,10 @@
       <c r="F41" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="2">
         <v>41513</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="2">
         <v>41516</v>
       </c>
       <c r="I41" s="118">
@@ -4115,10 +4131,10 @@
       <c r="F42" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="2">
         <v>41516</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="2">
         <v>41519</v>
       </c>
       <c r="I42" s="118">
@@ -4147,8 +4163,8 @@
       <c r="F43" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
       <c r="I43" s="118">
         <v>41521</v>
       </c>
@@ -4175,10 +4191,10 @@
       <c r="F44" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="2">
         <v>41516</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44" s="2">
         <v>41519</v>
       </c>
       <c r="I44" s="118">
@@ -4205,115 +4221,93 @@
         <v>10584</v>
       </c>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
       <c r="I45" s="118"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>158</v>
+        <v>89</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="126">
-        <v>5724</v>
+        <v>80</v>
+      </c>
+      <c r="E46" s="133">
+        <v>4489.5</v>
       </c>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
       <c r="I46" s="118"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>158</v>
+        <v>89</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="126">
-        <v>6372</v>
+        <v>177</v>
+      </c>
+      <c r="E47" s="133">
+        <v>7261.15</v>
       </c>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
       <c r="I47" s="118"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="E48" s="126">
-        <v>4163.04</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G48" s="1">
-        <v>41515</v>
-      </c>
-      <c r="H48" s="1">
-        <v>41518</v>
-      </c>
-      <c r="I48" s="118">
-        <v>41527</v>
-      </c>
-      <c r="J48" s="115" t="s">
-        <v>23</v>
-      </c>
+        <v>5724</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="118"/>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="E49" s="126">
-        <v>1214.22</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G49" s="1">
-        <v>41515</v>
-      </c>
-      <c r="H49" s="1">
-        <v>41518</v>
-      </c>
-      <c r="I49" s="118">
-        <v>41527</v>
-      </c>
-      <c r="J49" s="115" t="s">
-        <v>23</v>
-      </c>
+        <v>6372</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="118"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
@@ -4326,19 +4320,19 @@
         <v>89</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>17</v>
+        <v>169</v>
       </c>
       <c r="E50" s="126">
-        <v>2413.2399999999998</v>
+        <v>4163.04</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G50" s="1">
-        <v>41527</v>
-      </c>
-      <c r="H50" s="1">
-        <v>41530</v>
+        <v>170</v>
+      </c>
+      <c r="G50" s="2">
+        <v>41515</v>
+      </c>
+      <c r="H50" s="2">
+        <v>41518</v>
       </c>
       <c r="I50" s="118">
         <v>41527</v>
@@ -4358,84 +4352,94 @@
         <v>89</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>17</v>
+        <v>169</v>
       </c>
       <c r="E51" s="126">
-        <v>227.55</v>
+        <v>1214.22</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G51" s="1">
-        <v>41528</v>
-      </c>
-      <c r="H51" s="1">
-        <v>41531</v>
+        <v>171</v>
+      </c>
+      <c r="G51" s="2">
+        <v>41515</v>
+      </c>
+      <c r="H51" s="2">
+        <v>41518</v>
       </c>
       <c r="I51" s="118">
-        <v>41528</v>
+        <v>41527</v>
       </c>
       <c r="J51" s="115" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="126">
+        <v>2413.2399999999998</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G52" s="2">
+        <v>41527</v>
+      </c>
+      <c r="H52" s="2">
+        <v>41530</v>
+      </c>
+      <c r="I52" s="118">
+        <v>41527</v>
+      </c>
+      <c r="J52" s="115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B53" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="42" t="s">
+      <c r="C53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="122">
-        <v>247.93</v>
-      </c>
-      <c r="F52" t="s">
-        <v>175</v>
-      </c>
-      <c r="G52" s="2">
-        <v>41534</v>
-      </c>
-      <c r="H52" s="2">
-        <v>41537</v>
-      </c>
-      <c r="I52" s="119">
-        <v>41534</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="E53" s="126">
+        <v>227.55</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G53" s="2">
+        <v>41528</v>
+      </c>
+      <c r="H53" s="2">
+        <v>41531</v>
+      </c>
+      <c r="I53" s="118">
+        <v>41528</v>
+      </c>
+      <c r="J53" s="115" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="B53" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D53" t="s">
-        <v>176</v>
-      </c>
-      <c r="E53" s="122">
-        <v>360</v>
-      </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2">
-        <v>41537</v>
-      </c>
-      <c r="I53" s="119"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B54" s="42" t="s">
         <v>86</v>
@@ -4447,39 +4451,82 @@
         <v>17</v>
       </c>
       <c r="E54" s="122">
-        <v>257.38</v>
+        <v>247.93</v>
       </c>
       <c r="F54" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G54" s="2">
-        <v>41536</v>
+        <v>41534</v>
       </c>
       <c r="H54" s="2">
-        <v>41539</v>
-      </c>
-      <c r="I54" s="119" t="s">
-        <v>178</v>
+        <v>41537</v>
+      </c>
+      <c r="I54" s="119">
+        <v>41534</v>
       </c>
       <c r="J54" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="42"/>
-      <c r="B55" s="42"/>
-      <c r="C55" s="1"/>
+      <c r="A55" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="122">
+        <v>360</v>
+      </c>
       <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="119"/>
+      <c r="H55" s="2">
+        <v>41537</v>
+      </c>
+      <c r="I55" s="119">
+        <v>41537</v>
+      </c>
+      <c r="J55" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="42"/>
-      <c r="B56" s="42"/>
-      <c r="C56" s="1"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="119"/>
+      <c r="A56" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="122">
+        <v>257.38</v>
+      </c>
+      <c r="F56" t="s">
+        <v>176</v>
+      </c>
+      <c r="G56" s="2">
+        <v>41536</v>
+      </c>
+      <c r="H56" s="2">
+        <v>41539</v>
+      </c>
+      <c r="I56" s="119">
+        <v>41536</v>
+      </c>
+      <c r="J56" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="42"/>
@@ -4497,61 +4544,77 @@
       <c r="H58" s="2"/>
       <c r="I58" s="119"/>
     </row>
-    <row r="59" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A59" s="45" t="s">
+    <row r="59" spans="1:10">
+      <c r="A59" s="42"/>
+      <c r="B59" s="42"/>
+      <c r="C59" s="1"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="119"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="42"/>
+      <c r="B60" s="42"/>
+      <c r="C60" s="1"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="119"/>
+    </row>
+    <row r="61" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A61" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="45"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="127">
+      <c r="B61" s="45"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="127">
         <f>SUBTOTAL(109,[Kwota])</f>
-        <v>115547.1</v>
-      </c>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="120"/>
-      <c r="J59" s="116">
+        <v>127297.75</v>
+      </c>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="120"/>
+      <c r="J61" s="116">
         <f>SUBTOTAL(103,[Konto])</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" thickTop="1"/>
-    <row r="67" spans="1:10">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="125"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="121"/>
-      <c r="J67" s="112"/>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="125"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="121"/>
-      <c r="J84" s="112"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="125"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="121"/>
+      <c r="J69" s="112"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="125"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="121"/>
+      <c r="J86" s="112"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60:A67">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62:A69">
       <formula1>$M$4:$M$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B67 B22:B52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62:B69 B22:B54">
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A60">
       <formula1>$M$3:$M$18</formula1>
     </dataValidation>
   </dataValidations>
@@ -4568,7 +4631,7 @@
   <dimension ref="A3:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4679,7 +4742,7 @@
         <v>142</v>
       </c>
       <c r="B7" s="44">
-        <v>17100.03</v>
+        <v>15046.789999999999</v>
       </c>
       <c r="C7" s="44">
         <v>12140.82</v>
@@ -4688,14 +4751,16 @@
       <c r="E7" s="44"/>
       <c r="F7" s="44"/>
       <c r="G7" s="130">
-        <v>29240.85</v>
+        <v>27187.61</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="129" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="44"/>
+      <c r="B8" s="44">
+        <v>14669.199999999999</v>
+      </c>
       <c r="C8" s="44">
         <v>10584</v>
       </c>
@@ -4703,7 +4768,7 @@
       <c r="E8" s="44"/>
       <c r="F8" s="44"/>
       <c r="G8" s="130">
-        <v>10584</v>
+        <v>25253.199999999997</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4726,7 +4791,7 @@
         <v>165</v>
       </c>
       <c r="B10" s="44">
-        <v>52011.969999999994</v>
+        <v>64627.929999999993</v>
       </c>
       <c r="C10" s="44">
         <v>45404.82</v>
@@ -4741,7 +4806,7 @@
         <v>2526</v>
       </c>
       <c r="G10" s="131">
-        <v>114681.79</v>
+        <v>127297.74999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4755,7 +4820,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4870,6 +4935,9 @@
       <c r="F6" s="2">
         <v>41536</v>
       </c>
+      <c r="G6" s="2">
+        <v>41537</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -5032,9 +5100,7 @@
         <v>442800</v>
       </c>
       <c r="E19" s="132"/>
-      <c r="F19" s="1" t="s">
-        <v>169</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wstępnie zamknięcie etapu strop i schody
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="13020" windowHeight="2895"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13020" windowHeight="2895" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wydatki budowa" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="12" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -862,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1003,11 +1003,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
     <dxf>
       <font>
         <b/>
@@ -1017,6 +1018,9 @@
       <font>
         <color theme="3"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1340,7 +1344,14 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1580,6 +1591,45 @@
                 <c:pt idx="1">
                   <c:v>9100</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>-18200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-47500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-21600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-45700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-16200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-22200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-39900</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-31300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-20000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-31600</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1668,7 +1718,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="41538.576876388892" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="59">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="41538.585481944443" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="59">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabela1"/>
   </cacheSource>
@@ -2244,7 +2294,7 @@
     <x v="4"/>
     <s v="Antoni Nowak"/>
     <s v="Strop"/>
-    <n v="10584"/>
+    <n v="10000"/>
     <m/>
     <m/>
     <m/>
@@ -2435,7 +2485,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -2528,14 +2578,14 @@
     <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="17">
+    <format dxfId="19">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="18">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2557,16 +2607,16 @@
     <sortCondition ref="A1:A52"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="11"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="10"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="9"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="7"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="6"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="5"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="19" totalsRowDxfId="3"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="18" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="12"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="11"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="10"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="9"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="7"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="6"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="5"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="21" totalsRowDxfId="4"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="20" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2584,10 +2634,10 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="15">
+    <tableColumn id="4" name="Plan suma" dataDxfId="2">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Rzecz różnica" dataDxfId="14"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="17"/>
     <tableColumn id="7" name="Plan"/>
     <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
@@ -2885,9 +2935,9 @@
   </sheetPr>
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4218,7 +4268,7 @@
         <v>29</v>
       </c>
       <c r="E45" s="126">
-        <v>10584</v>
+        <v>10000</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="2"/>
@@ -4569,7 +4619,7 @@
       <c r="D61" s="45"/>
       <c r="E61" s="127">
         <f>SUBTOTAL(109,[Kwota])</f>
-        <v>127297.75</v>
+        <v>126713.75</v>
       </c>
       <c r="F61" s="45"/>
       <c r="G61" s="45"/>
@@ -4631,7 +4681,7 @@
   <dimension ref="A3:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4762,13 +4812,13 @@
         <v>14669.199999999999</v>
       </c>
       <c r="C8" s="44">
-        <v>10584</v>
+        <v>10000</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="44"/>
       <c r="F8" s="44"/>
       <c r="G8" s="130">
-        <v>25253.199999999997</v>
+        <v>24669.199999999997</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4794,7 +4844,7 @@
         <v>64627.929999999993</v>
       </c>
       <c r="C10" s="44">
-        <v>45404.82</v>
+        <v>44820.82</v>
       </c>
       <c r="D10" s="44">
         <v>9542</v>
@@ -4806,7 +4856,7 @@
         <v>2526</v>
       </c>
       <c r="G10" s="131">
-        <v>127297.74999999999</v>
+        <v>126713.74999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4819,8 +4869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4927,11 +4977,17 @@
       <c r="B6">
         <v>43200</v>
       </c>
+      <c r="C6" s="134">
+        <v>25000</v>
+      </c>
       <c r="D6" s="44">
         <f>Tabela5[[#This Row],[Planowane]]+D5</f>
         <v>118600</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-18200</v>
+      </c>
       <c r="F6" s="2">
         <v>41536</v>
       </c>
@@ -4950,7 +5006,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D6</f>
         <v>166100</v>
       </c>
-      <c r="E7" s="44"/>
+      <c r="E7" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-47500</v>
+      </c>
       <c r="F7" s="2">
         <v>41571</v>
       </c>
@@ -4966,7 +5025,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D7</f>
         <v>198100</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-32000</v>
+      </c>
       <c r="F8" s="44"/>
     </row>
     <row r="9" spans="1:7">
@@ -4980,7 +5042,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D8</f>
         <v>219700</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-21600</v>
+      </c>
       <c r="F9" s="44"/>
     </row>
     <row r="10" spans="1:7">
@@ -4994,6 +5059,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D9</f>
         <v>229400</v>
       </c>
+      <c r="E10" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-9700</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
@@ -5006,6 +5075,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D10</f>
         <v>275100</v>
       </c>
+      <c r="E11" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-45700</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
@@ -5018,6 +5091,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D11</f>
         <v>291300</v>
       </c>
+      <c r="E12" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-16200</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
@@ -5030,6 +5107,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D12</f>
         <v>313500</v>
       </c>
+      <c r="E13" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-22200</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -5042,6 +5123,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D13</f>
         <v>353400</v>
       </c>
+      <c r="E14" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-39900</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -5054,6 +5139,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D14</f>
         <v>359900</v>
       </c>
+      <c r="E15" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-6500</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -5066,6 +5155,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D15</f>
         <v>391200</v>
       </c>
+      <c r="E16" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-31300</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
@@ -5078,6 +5171,10 @@
         <f>Tabela5[[#This Row],[Planowane]]+D16</f>
         <v>411200</v>
       </c>
+      <c r="E17" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-20000</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
@@ -5089,6 +5186,10 @@
       <c r="D18" s="44">
         <f>Tabela5[[#This Row],[Planowane]]+D17</f>
         <v>442800</v>
+      </c>
+      <c r="E18" s="44">
+        <f>Tabela5[[#This Row],[Rzeczywiste]]-Tabela5[[#This Row],[Planowane]]</f>
+        <v>-31600</v>
       </c>
     </row>
     <row r="19" spans="1:7">

</xml_diff>

<commit_message>
faktury Manex za poddasze
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="183">
   <si>
     <t>Opis</t>
   </si>
@@ -567,6 +567,12 @@
   </si>
   <si>
     <t>6199/T/09/2013</t>
+  </si>
+  <si>
+    <t>Stal piętro</t>
+  </si>
+  <si>
+    <t>6284/T/09/2013</t>
   </si>
 </sst>
 </file>
@@ -1010,22 +1016,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1058,11 +1048,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1091,17 +1076,6 @@
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FFC00000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1229,9 +1203,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1354,6 +1325,41 @@
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1604,25 +1610,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62720256"/>
-        <c:axId val="62738432"/>
+        <c:axId val="63113472"/>
+        <c:axId val="63131648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62720256"/>
+        <c:axId val="63113472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62738432"/>
+        <c:crossAx val="63131648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62738432"/>
+        <c:axId val="63131648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1631,7 +1637,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62720256"/>
+        <c:crossAx val="63113472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1644,7 +1650,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2546,14 +2552,14 @@
     <dataField name="Suma z Kwota" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="13">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="12">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2562,8 +2568,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J63" totalsRowCount="1">
-  <autoFilter ref="A1:J62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J64" totalsRowCount="1">
+  <autoFilter ref="A1:J63">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
@@ -2575,16 +2581,16 @@
     <sortCondition ref="A62"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="16"/>
-    <tableColumn id="9" name="Typ" totalsRowDxfId="15"/>
-    <tableColumn id="10" name="Dostawca" totalsRowDxfId="14"/>
-    <tableColumn id="5" name="Opis" totalsRowDxfId="13"/>
-    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="10"/>
-    <tableColumn id="8" name="Data faktury" totalsRowDxfId="9"/>
-    <tableColumn id="11" name="Data płatności" totalsRowDxfId="8"/>
-    <tableColumn id="6" name="Zapłacono" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Etap" totalsRowLabel="Suma" totalsRowDxfId="9"/>
+    <tableColumn id="9" name="Typ" totalsRowDxfId="8"/>
+    <tableColumn id="10" name="Dostawca" totalsRowDxfId="7"/>
+    <tableColumn id="5" name="Opis" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="Kwota" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Faktura numer" totalsRowDxfId="4"/>
+    <tableColumn id="8" name="Data faktury" totalsRowDxfId="3"/>
+    <tableColumn id="11" name="Data płatności" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Zapłacono" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="7" name="Konto" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2602,10 +2608,10 @@
     <tableColumn id="1" name="Kolumna1"/>
     <tableColumn id="2" name="Planowane"/>
     <tableColumn id="3" name="Rzeczywiste"/>
-    <tableColumn id="4" name="Plan suma" dataDxfId="1">
+    <tableColumn id="4" name="Plan suma" dataDxfId="11">
       <calculatedColumnFormula>Tabela5[[#This Row],[Planowane]]+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Rzecz różnica" dataDxfId="0"/>
+    <tableColumn id="6" name="Rzecz różnica" dataDxfId="10"/>
     <tableColumn id="7" name="Plan"/>
     <tableColumn id="5" name="Realizacja"/>
   </tableColumns>
@@ -2901,11 +2907,11 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M88"/>
+  <dimension ref="A1:M89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50:XFD51"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4370,29 +4376,40 @@
       <c r="H49" s="2">
         <v>41547</v>
       </c>
-      <c r="I49" s="119"/>
+      <c r="I49" s="119">
+        <v>41547</v>
+      </c>
+      <c r="J49" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50" s="126">
-        <v>10100</v>
-      </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="118">
-        <v>41542</v>
+      <c r="A50" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" t="s">
+        <v>181</v>
+      </c>
+      <c r="E50" s="122">
+        <v>594.69000000000005</v>
+      </c>
+      <c r="F50" t="s">
+        <v>182</v>
+      </c>
+      <c r="G50" s="2">
+        <v>41547</v>
+      </c>
+      <c r="H50" s="2">
+        <v>41550</v>
+      </c>
+      <c r="I50" s="119">
+        <v>41547</v>
       </c>
       <c r="J50" t="s">
         <v>23</v>
@@ -4403,28 +4420,22 @@
         <v>143</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E51" s="133">
-        <v>4489.5</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G51" s="2">
-        <v>41511</v>
-      </c>
-      <c r="H51" s="2">
-        <v>41514</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E51" s="126">
+        <v>10100</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
       <c r="I51" s="118">
-        <v>41511</v>
+        <v>41542</v>
       </c>
       <c r="J51" t="s">
         <v>23</v>
@@ -4441,22 +4452,22 @@
         <v>89</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>177</v>
+        <v>80</v>
       </c>
       <c r="E52" s="133">
-        <v>7792.51</v>
+        <v>4489.5</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G52" s="2">
-        <v>41533</v>
+        <v>41542</v>
       </c>
       <c r="H52" s="2">
-        <v>41536</v>
+        <v>41545</v>
       </c>
       <c r="I52" s="118">
-        <v>41541</v>
+        <v>41542</v>
       </c>
       <c r="J52" t="s">
         <v>23</v>
@@ -4473,56 +4484,56 @@
         <v>89</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E53" s="133">
+        <v>7792.51</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G53" s="2">
+        <v>41533</v>
+      </c>
+      <c r="H53" s="2">
+        <v>41536</v>
+      </c>
+      <c r="I53" s="118">
+        <v>41541</v>
+      </c>
+      <c r="J53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="126">
+      <c r="E54" s="126">
         <v>2413.2399999999998</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G54" s="2">
         <v>41527</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H54" s="2">
         <v>41530</v>
       </c>
-      <c r="I53" s="118">
+      <c r="I54" s="118">
         <v>41527</v>
       </c>
-      <c r="J53" s="115" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="B54" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54" s="122">
-        <v>247.93</v>
-      </c>
-      <c r="F54" t="s">
-        <v>174</v>
-      </c>
-      <c r="G54" s="2">
-        <v>41534</v>
-      </c>
-      <c r="H54" s="2">
-        <v>41537</v>
-      </c>
-      <c r="I54" s="119">
-        <v>41534</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="J54" s="115" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4540,44 +4551,55 @@
         <v>17</v>
       </c>
       <c r="E55" s="122">
-        <v>257.38</v>
+        <v>247.93</v>
       </c>
       <c r="F55" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G55" s="2">
-        <v>41536</v>
+        <v>41534</v>
       </c>
       <c r="H55" s="2">
-        <v>41539</v>
+        <v>41537</v>
       </c>
       <c r="I55" s="119">
-        <v>41536</v>
+        <v>41534</v>
       </c>
       <c r="J55" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="126">
-        <v>5724</v>
-      </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="118"/>
+      <c r="A56" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="122">
+        <v>257.38</v>
+      </c>
+      <c r="F56" t="s">
+        <v>176</v>
+      </c>
+      <c r="G56" s="2">
+        <v>41536</v>
+      </c>
+      <c r="H56" s="2">
+        <v>41539</v>
+      </c>
+      <c r="I56" s="119">
+        <v>41536</v>
+      </c>
+      <c r="J56" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
@@ -4590,10 +4612,10 @@
         <v>158</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E57" s="126">
-        <v>6372</v>
+        <v>5724</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="2"/>
@@ -4601,12 +4623,25 @@
       <c r="I57" s="118"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="42"/>
-      <c r="B58" s="42"/>
-      <c r="C58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="126">
+        <v>6372</v>
+      </c>
+      <c r="F58" s="1"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="I58" s="119"/>
+      <c r="I58" s="118"/>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="42"/>
@@ -4640,61 +4675,69 @@
       <c r="H62" s="2"/>
       <c r="I62" s="119"/>
     </row>
-    <row r="63" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A63" s="45" t="s">
+    <row r="63" spans="1:10">
+      <c r="A63" s="42"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="1"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="119"/>
+    </row>
+    <row r="64" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A64" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B63" s="45"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="127">
+      <c r="B64" s="45"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="127">
         <f>SUBTOTAL(109,[Kwota])</f>
-        <v>130131.51</v>
-      </c>
-      <c r="F63" s="45"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="120"/>
-      <c r="J63" s="116">
+        <v>130726.2</v>
+      </c>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="120"/>
+      <c r="J64" s="116">
         <f>SUBTOTAL(103,[Konto])</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" thickTop="1"/>
-    <row r="71" spans="1:10">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="125"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="121"/>
-      <c r="J71" s="112"/>
-    </row>
-    <row r="88" spans="1:10">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="125"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="121"/>
-      <c r="J88" s="112"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="72" spans="1:10">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="125"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="121"/>
+      <c r="J72" s="112"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="125"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="121"/>
+      <c r="J89" s="112"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A64:A71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A65:A72">
       <formula1>$M$4:$M$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64:B71 B22:B54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B65:B72 B22:B55">
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A62">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A63">
       <formula1>$M$3:$M$18</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
zwrot fakro, faktury zgk
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki budowa.xlsx
+++ b/plan/Mati - wydatki budowa.xlsx
@@ -29,7 +29,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="F42" authorId="0">
+    <comment ref="F43" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0">
+    <comment ref="F46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="0">
+    <comment ref="F47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F81" authorId="0">
+    <comment ref="F82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F100" authorId="0">
+    <comment ref="F102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F102" authorId="0">
+    <comment ref="F104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F109" authorId="0">
+    <comment ref="F111" authorId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F112" authorId="0">
+    <comment ref="F114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="270">
   <si>
     <t>Opis</t>
   </si>
@@ -993,9 +993,6 @@
     <t>Zajęcia pasa ruchu</t>
   </si>
   <si>
-    <t>Opłata przyłączeniowa</t>
-  </si>
-  <si>
     <t>Prokad</t>
   </si>
   <si>
@@ -1017,9 +1014,6 @@
     <t>Umieszczenie przyłacza. Opłata roczna</t>
   </si>
   <si>
-    <t>Opłata za odebranie przyłączy</t>
-  </si>
-  <si>
     <t>Kaucja za worki</t>
   </si>
   <si>
@@ -1027,6 +1021,24 @@
   </si>
   <si>
     <t>SB/003383</t>
+  </si>
+  <si>
+    <t>Odbiór przyłącza wod-kan</t>
+  </si>
+  <si>
+    <t>ZGK Kąty</t>
+  </si>
+  <si>
+    <t>Wpięcie przył. kan.</t>
+  </si>
+  <si>
+    <t>Wpięcie przył. wod.</t>
+  </si>
+  <si>
+    <t>Fakro</t>
+  </si>
+  <si>
+    <t>Zwrot - Okna promocja</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1467,6 +1479,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2076,25 +2089,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62839040"/>
-        <c:axId val="63713280"/>
+        <c:axId val="62707968"/>
+        <c:axId val="63578112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62839040"/>
+        <c:axId val="62707968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63713280"/>
+        <c:crossAx val="63578112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63713280"/>
+        <c:axId val="63578112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2116,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62839040"/>
+        <c:crossAx val="62707968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2116,7 +2129,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000633" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000633" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000655" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000655" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3684,8 +3697,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J119" totalsRowCount="1">
-  <autoFilter ref="A1:J118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J121" totalsRowCount="1">
+  <autoFilter ref="A1:J120">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
@@ -4024,11 +4037,11 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M144"/>
+  <dimension ref="A1:M146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K99" sqref="K99"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4728,16 +4741,23 @@
         <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E24" s="123"/>
+        <v>253</v>
+      </c>
+      <c r="E24" s="123">
+        <v>36</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="116"/>
+      <c r="I24" s="116">
+        <v>41605</v>
+      </c>
+      <c r="J24" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
@@ -4747,16 +4767,23 @@
         <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E25" s="123"/>
+        <v>260</v>
+      </c>
+      <c r="E25" s="123">
+        <v>22.19</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="116"/>
+      <c r="I25" s="116">
+        <v>41605</v>
+      </c>
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
@@ -4766,19 +4793,23 @@
         <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="E26" s="123">
-        <v>36</v>
+        <v>184.5</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="G26" s="130">
+        <v>41603</v>
+      </c>
+      <c r="H26" s="130">
+        <v>41617</v>
+      </c>
       <c r="I26" s="116">
-        <v>41605</v>
+        <v>41606</v>
       </c>
       <c r="J26" t="s">
         <v>23</v>
@@ -4792,19 +4823,23 @@
         <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="E27" s="123">
-        <v>22.19</v>
+        <v>387.45</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="G27" s="130">
+        <v>41603</v>
+      </c>
+      <c r="H27" s="130">
+        <v>41617</v>
+      </c>
       <c r="I27" s="116">
-        <v>41605</v>
+        <v>41606</v>
       </c>
       <c r="J27" t="s">
         <v>23</v>
@@ -4812,28 +4847,32 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>103</v>
+        <v>265</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>78</v>
+        <v>266</v>
       </c>
       <c r="E28" s="123">
-        <v>400</v>
+        <v>159.9</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="130">
+        <v>41603</v>
+      </c>
+      <c r="H28" s="130">
+        <v>41617</v>
+      </c>
       <c r="I28" s="116">
-        <v>41474</v>
-      </c>
-      <c r="J28" s="113" t="s">
-        <v>84</v>
+        <v>41606</v>
+      </c>
+      <c r="J28" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -4847,10 +4886,10 @@
         <v>103</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" s="123">
-        <v>650</v>
+        <v>400</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
@@ -4867,16 +4906,16 @@
         <v>141</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="E30" s="123">
-        <v>7800</v>
+        <v>650</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
@@ -4896,28 +4935,22 @@
         <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E31" s="123">
-        <v>1510.21</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="2">
-        <v>41494</v>
-      </c>
-      <c r="H31" s="2">
-        <v>41497</v>
-      </c>
+        <v>7800</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="116">
-        <v>41495</v>
+        <v>41474</v>
       </c>
       <c r="J31" s="113" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -4931,25 +4964,25 @@
         <v>89</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E32" s="123">
-        <v>5878.78</v>
+        <v>1510.21</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G32" s="2">
         <v>41494</v>
       </c>
       <c r="H32" s="2">
-        <v>41501</v>
+        <v>41497</v>
       </c>
       <c r="I32" s="116">
-        <v>41501</v>
+        <v>41495</v>
       </c>
       <c r="J32" s="113" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -4963,16 +4996,16 @@
         <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E33" s="123">
-        <v>19.079999999999998</v>
+        <v>5878.78</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G33" s="2">
-        <v>41498</v>
+        <v>41494</v>
       </c>
       <c r="H33" s="2">
         <v>41501</v>
@@ -4995,13 +5028,13 @@
         <v>89</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E34" s="123">
-        <v>115.01</v>
+        <v>19.079999999999998</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G34" s="2">
         <v>41498</v>
@@ -5027,19 +5060,19 @@
         <v>89</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E35" s="123">
-        <v>8280.36</v>
+        <v>115.01</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G35" s="2">
-        <v>41499</v>
+        <v>41498</v>
       </c>
       <c r="H35" s="2">
-        <v>41502</v>
+        <v>41501</v>
       </c>
       <c r="I35" s="116">
         <v>41501</v>
@@ -5059,22 +5092,22 @@
         <v>89</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E36" s="123">
-        <v>1657.43</v>
+        <v>8280.36</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G36" s="2">
+        <v>41499</v>
+      </c>
+      <c r="H36" s="2">
         <v>41502</v>
       </c>
-      <c r="H36" s="2">
-        <v>41505</v>
-      </c>
       <c r="I36" s="116">
-        <v>41502</v>
+        <v>41501</v>
       </c>
       <c r="J36" s="113" t="s">
         <v>23</v>
@@ -5094,19 +5127,19 @@
         <v>17</v>
       </c>
       <c r="E37" s="123">
-        <v>512.29999999999995</v>
+        <v>1657.43</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G37" s="2">
         <v>41502</v>
       </c>
       <c r="H37" s="2">
-        <v>41509</v>
+        <v>41505</v>
       </c>
       <c r="I37" s="116">
-        <v>41507</v>
+        <v>41502</v>
       </c>
       <c r="J37" s="113" t="s">
         <v>23</v>
@@ -5117,22 +5150,26 @@
         <v>141</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E38" s="123">
-        <v>10584</v>
+        <v>512.29999999999995</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="G38" s="2">
+        <v>41502</v>
+      </c>
+      <c r="H38" s="2">
+        <v>41509</v>
+      </c>
       <c r="I38" s="116">
         <v>41507</v>
       </c>
@@ -5145,28 +5182,24 @@
         <v>141</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="E39" s="123">
-        <v>7610.63</v>
+        <v>10584</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G39" s="2">
-        <v>41514</v>
-      </c>
-      <c r="H39" s="2">
-        <v>41517</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
       <c r="I39" s="116">
-        <v>41515</v>
+        <v>41507</v>
       </c>
       <c r="J39" s="113" t="s">
         <v>23</v>
@@ -5183,22 +5216,22 @@
         <v>89</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="E40" s="123">
-        <v>992.96</v>
+        <v>7610.63</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G40" s="2">
-        <v>41492</v>
+        <v>41514</v>
       </c>
       <c r="H40" s="2">
-        <v>41495</v>
+        <v>41517</v>
       </c>
       <c r="I40" s="116">
-        <v>41516</v>
+        <v>41515</v>
       </c>
       <c r="J40" s="113" t="s">
         <v>23</v>
@@ -5212,56 +5245,56 @@
         <v>86</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="E41" s="123">
-        <v>335.18</v>
+        <v>992.96</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="G41" s="2">
+        <v>41492</v>
+      </c>
+      <c r="H41" s="2">
+        <v>41495</v>
+      </c>
       <c r="I41" s="116">
-        <v>41521</v>
+        <v>41516</v>
       </c>
       <c r="J41" s="113" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
-        <v>205</v>
+        <v>141</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>194</v>
+        <v>34</v>
       </c>
       <c r="E42" s="123">
-        <v>1764.84</v>
+        <v>335.18</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G42" s="2">
-        <v>41570</v>
-      </c>
-      <c r="H42" s="2">
-        <v>41573</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
       <c r="I42" s="116">
-        <v>41570</v>
-      </c>
-      <c r="J42" t="s">
-        <v>23</v>
+        <v>41521</v>
+      </c>
+      <c r="J42" s="113" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -5275,13 +5308,13 @@
         <v>89</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E43" s="123">
-        <v>241.71</v>
+        <v>1764.84</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G43" s="2">
         <v>41570</v>
@@ -5304,19 +5337,25 @@
         <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>203</v>
+        <v>89</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E44" s="123">
-        <v>700</v>
-      </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+        <v>241.71</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G44" s="2">
+        <v>41570</v>
+      </c>
+      <c r="H44" s="2">
+        <v>41573</v>
+      </c>
       <c r="I44" s="116">
-        <v>41571</v>
+        <v>41570</v>
       </c>
       <c r="J44" t="s">
         <v>23</v>
@@ -5330,25 +5369,19 @@
         <v>86</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>89</v>
+        <v>203</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E45" s="123">
-        <v>69.88</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G45" s="2">
-        <v>41570</v>
-      </c>
-      <c r="H45" s="2">
-        <v>41573</v>
-      </c>
+        <v>700</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
       <c r="I45" s="116">
-        <v>41570</v>
+        <v>41571</v>
       </c>
       <c r="J45" t="s">
         <v>23</v>
@@ -5365,22 +5398,22 @@
         <v>89</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="E46" s="123">
-        <v>40.619999999999997</v>
+        <v>69.88</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="G46" s="2">
-        <v>41582</v>
+        <v>41570</v>
       </c>
       <c r="H46" s="2">
-        <v>41585</v>
+        <v>41573</v>
       </c>
       <c r="I46" s="116">
-        <v>41582</v>
+        <v>41570</v>
       </c>
       <c r="J46" t="s">
         <v>23</v>
@@ -5391,25 +5424,31 @@
         <v>205</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="E47" s="123">
-        <v>3800</v>
-      </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+        <v>40.619999999999997</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G47" s="2">
+        <v>41582</v>
+      </c>
+      <c r="H47" s="2">
+        <v>41585</v>
+      </c>
       <c r="I47" s="116">
-        <v>41585</v>
+        <v>41582</v>
       </c>
       <c r="J47" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -5417,16 +5456,16 @@
         <v>205</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E48" s="123">
-        <v>400</v>
+        <v>3800</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="2"/>
@@ -5449,10 +5488,10 @@
         <v>35</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>233</v>
+        <v>8</v>
       </c>
       <c r="E49" s="123">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="2"/>
@@ -5472,28 +5511,22 @@
         <v>86</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E50" s="123">
-        <v>118.51</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G50" s="2">
+        <v>450</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="116">
         <v>41585</v>
       </c>
-      <c r="H50" s="2">
-        <v>41588</v>
-      </c>
-      <c r="I50" s="116">
-        <v>41586</v>
-      </c>
       <c r="J50" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -5504,19 +5537,25 @@
         <v>86</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>245</v>
+        <v>89</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E51" s="123">
-        <v>1080</v>
-      </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+        <v>118.51</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G51" s="2">
+        <v>41585</v>
+      </c>
+      <c r="H51" s="2">
+        <v>41588</v>
+      </c>
       <c r="I51" s="116">
-        <v>41598</v>
+        <v>41586</v>
       </c>
       <c r="J51" t="s">
         <v>23</v>
@@ -5533,10 +5572,10 @@
         <v>245</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="E52" s="123">
-        <v>100</v>
+        <v>1080</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="2"/>
@@ -5550,33 +5589,27 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>89</v>
+        <v>245</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>104</v>
+        <v>261</v>
       </c>
       <c r="E53" s="123">
-        <v>3813.05</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G53" s="2">
-        <v>41512</v>
-      </c>
-      <c r="H53" s="2">
-        <v>41519</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
       <c r="I53" s="116">
-        <v>41515</v>
-      </c>
-      <c r="J53" s="113" t="s">
+        <v>41598</v>
+      </c>
+      <c r="J53" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5591,19 +5624,19 @@
         <v>89</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E54" s="123">
-        <v>66.180000000000007</v>
+        <v>3813.05</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G54" s="2">
-        <v>41513</v>
+        <v>41512</v>
       </c>
       <c r="H54" s="2">
-        <v>41516</v>
+        <v>41519</v>
       </c>
       <c r="I54" s="116">
         <v>41515</v>
@@ -5623,13 +5656,13 @@
         <v>89</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E55" s="123">
-        <v>649.32000000000005</v>
+        <v>66.180000000000007</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G55" s="2">
         <v>41513</v>
@@ -5655,22 +5688,22 @@
         <v>89</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E56" s="123">
-        <v>3084.07</v>
+        <v>649.32000000000005</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G56" s="2">
+        <v>41513</v>
+      </c>
+      <c r="H56" s="2">
         <v>41516</v>
       </c>
-      <c r="H56" s="2">
-        <v>41519</v>
-      </c>
       <c r="I56" s="116">
-        <v>41516</v>
+        <v>41515</v>
       </c>
       <c r="J56" s="113" t="s">
         <v>23</v>
@@ -5681,27 +5714,31 @@
         <v>206</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="E57" s="123">
-        <v>7010.82</v>
+        <v>3084.07</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="G57" s="2">
+        <v>41516</v>
+      </c>
+      <c r="H57" s="2">
+        <v>41519</v>
+      </c>
       <c r="I57" s="116">
-        <v>41521</v>
+        <v>41516</v>
       </c>
       <c r="J57" s="113" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -5709,19 +5746,19 @@
         <v>206</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>149</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="E58" s="123">
-        <v>54</v>
+        <v>7010.82</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -5740,28 +5777,24 @@
         <v>86</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E59" s="123">
-        <v>1415.36</v>
+        <v>54</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G59" s="2">
-        <v>41516</v>
-      </c>
-      <c r="H59" s="2">
-        <v>41519</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
       <c r="I59" s="116">
         <v>41521</v>
       </c>
       <c r="J59" s="113" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -5775,22 +5808,22 @@
         <v>89</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E60" s="123">
-        <v>4163.04</v>
+        <v>1415.36</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G60" s="2">
-        <v>41515</v>
+        <v>41516</v>
       </c>
       <c r="H60" s="2">
-        <v>41518</v>
+        <v>41519</v>
       </c>
       <c r="I60" s="116">
-        <v>41527</v>
+        <v>41521</v>
       </c>
       <c r="J60" s="113" t="s">
         <v>23</v>
@@ -5810,10 +5843,10 @@
         <v>160</v>
       </c>
       <c r="E61" s="123">
-        <v>1214.22</v>
+        <v>4163.04</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G61" s="2">
         <v>41515</v>
@@ -5839,22 +5872,22 @@
         <v>89</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="E62" s="123">
-        <v>227.55</v>
+        <v>1214.22</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G62" s="2">
-        <v>41528</v>
+        <v>41515</v>
       </c>
       <c r="H62" s="2">
-        <v>41531</v>
+        <v>41518</v>
       </c>
       <c r="I62" s="116">
-        <v>41528</v>
+        <v>41527</v>
       </c>
       <c r="J62" s="113" t="s">
         <v>23</v>
@@ -5868,21 +5901,25 @@
         <v>86</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="E63" s="123">
-        <v>360</v>
-      </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="2"/>
+        <v>227.55</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G63" s="2">
+        <v>41528</v>
+      </c>
       <c r="H63" s="2">
-        <v>41537</v>
+        <v>41531</v>
       </c>
       <c r="I63" s="116">
-        <v>41537</v>
+        <v>41528</v>
       </c>
       <c r="J63" s="113" t="s">
         <v>23</v>
@@ -5896,25 +5933,21 @@
         <v>86</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E64" s="123">
-        <v>2786.4</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G64" s="2">
-        <v>41544</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="2"/>
       <c r="H64" s="2">
-        <v>41547</v>
+        <v>41537</v>
       </c>
       <c r="I64" s="116">
-        <v>41547</v>
+        <v>41537</v>
       </c>
       <c r="J64" s="113" t="s">
         <v>23</v>
@@ -5931,19 +5964,19 @@
         <v>89</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E65" s="123">
-        <v>594.69000000000005</v>
+        <v>2786.4</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G65" s="2">
+        <v>41544</v>
+      </c>
+      <c r="H65" s="2">
         <v>41547</v>
-      </c>
-      <c r="H65" s="2">
-        <v>41550</v>
       </c>
       <c r="I65" s="116">
         <v>41547</v>
@@ -5957,27 +5990,31 @@
         <v>206</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="E66" s="123">
-        <v>2960</v>
+        <v>594.69000000000005</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="G66" s="2">
+        <v>41547</v>
+      </c>
+      <c r="H66" s="2">
+        <v>41550</v>
+      </c>
       <c r="I66" s="116">
-        <v>41552</v>
+        <v>41547</v>
       </c>
       <c r="J66" s="113" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -5985,26 +6022,22 @@
         <v>206</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>149</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="E67" s="123">
-        <v>200</v>
+        <v>2960</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G67" s="2">
-        <v>41549</v>
-      </c>
-      <c r="H67" s="2">
-        <v>41549</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
       <c r="I67" s="116">
         <v>41552</v>
       </c>
@@ -6023,19 +6056,19 @@
         <v>149</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E68" s="123">
-        <v>48.18</v>
+        <v>200</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G68" s="2">
-        <v>41548</v>
+        <v>41549</v>
       </c>
       <c r="H68" s="2">
-        <v>41548</v>
+        <v>41549</v>
       </c>
       <c r="I68" s="116">
         <v>41552</v>
@@ -6055,19 +6088,19 @@
         <v>149</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E69" s="123">
-        <v>90</v>
+        <v>48.18</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G69" s="2">
-        <v>41547</v>
+        <v>41548</v>
       </c>
       <c r="H69" s="2">
-        <v>41547</v>
+        <v>41548</v>
       </c>
       <c r="I69" s="116">
         <v>41552</v>
@@ -6081,26 +6114,30 @@
         <v>206</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>149</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="E70" s="123">
-        <v>2000</v>
+        <v>90</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="G70" s="2">
+        <v>41547</v>
+      </c>
+      <c r="H70" s="2">
+        <v>41547</v>
+      </c>
       <c r="I70" s="116">
-        <v>41578</v>
-      </c>
-      <c r="J70" t="s">
+        <v>41552</v>
+      </c>
+      <c r="J70" s="113" t="s">
         <v>84</v>
       </c>
     </row>
@@ -6109,27 +6146,27 @@
         <v>206</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>191</v>
+        <v>31</v>
       </c>
       <c r="E71" s="123">
-        <v>1260.76</v>
+        <v>2000</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>192</v>
+        <v>144</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="116">
-        <v>41557</v>
-      </c>
-      <c r="J71" s="113" t="s">
-        <v>23</v>
+        <v>41578</v>
+      </c>
+      <c r="J71" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -6143,22 +6180,18 @@
         <v>89</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>104</v>
+        <v>191</v>
       </c>
       <c r="E72" s="123">
-        <v>2398.8000000000002</v>
+        <v>1260.76</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G72" s="2">
-        <v>41558</v>
-      </c>
-      <c r="H72" s="2">
-        <v>41561</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
       <c r="I72" s="116">
-        <v>41558</v>
+        <v>41557</v>
       </c>
       <c r="J72" s="113" t="s">
         <v>23</v>
@@ -6169,62 +6202,62 @@
         <v>206</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>231</v>
+        <v>104</v>
       </c>
       <c r="E73" s="123">
-        <v>120</v>
-      </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
+        <v>2398.8000000000002</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G73" s="2">
+        <v>41558</v>
+      </c>
+      <c r="H73" s="2">
+        <v>41561</v>
+      </c>
       <c r="I73" s="116">
-        <v>41585</v>
-      </c>
-      <c r="J73" t="s">
-        <v>84</v>
+        <v>41558</v>
+      </c>
+      <c r="J73" s="113" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E74" s="123">
-        <v>192.4</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G74" s="2">
-        <v>41583</v>
-      </c>
-      <c r="H74" s="2">
-        <v>41586</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F74" s="1"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
       <c r="I74" s="116">
-        <v>41586</v>
+        <v>41585</v>
       </c>
       <c r="J74" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>86</v>
@@ -6233,24 +6266,24 @@
         <v>89</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>17</v>
+        <v>234</v>
       </c>
       <c r="E75" s="123">
-        <v>2413.2399999999998</v>
+        <v>192.4</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>163</v>
+        <v>235</v>
       </c>
       <c r="G75" s="2">
-        <v>41527</v>
+        <v>41583</v>
       </c>
       <c r="H75" s="2">
-        <v>41530</v>
+        <v>41586</v>
       </c>
       <c r="I75" s="116">
-        <v>41527</v>
-      </c>
-      <c r="J75" s="113" t="s">
+        <v>41586</v>
+      </c>
+      <c r="J75" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6268,19 +6301,19 @@
         <v>17</v>
       </c>
       <c r="E76" s="123">
-        <v>247.93</v>
+        <v>2413.2399999999998</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G76" s="2">
-        <v>41534</v>
+        <v>41527</v>
       </c>
       <c r="H76" s="2">
-        <v>41537</v>
+        <v>41530</v>
       </c>
       <c r="I76" s="116">
-        <v>41534</v>
+        <v>41527</v>
       </c>
       <c r="J76" s="113" t="s">
         <v>23</v>
@@ -6300,19 +6333,19 @@
         <v>17</v>
       </c>
       <c r="E77" s="123">
-        <v>257.38</v>
+        <v>247.93</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G77" s="2">
-        <v>41536</v>
+        <v>41534</v>
       </c>
       <c r="H77" s="2">
-        <v>41539</v>
+        <v>41537</v>
       </c>
       <c r="I77" s="116">
-        <v>41536</v>
+        <v>41534</v>
       </c>
       <c r="J77" s="113" t="s">
         <v>23</v>
@@ -6329,22 +6362,22 @@
         <v>89</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="E78" s="123">
-        <v>7792.51</v>
+        <v>257.38</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G78" s="2">
-        <v>41533</v>
+        <v>41536</v>
       </c>
       <c r="H78" s="2">
+        <v>41539</v>
+      </c>
+      <c r="I78" s="116">
         <v>41536</v>
-      </c>
-      <c r="I78" s="116">
-        <v>41541</v>
       </c>
       <c r="J78" s="113" t="s">
         <v>23</v>
@@ -6355,22 +6388,28 @@
         <v>207</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="E79" s="123">
-        <v>10100</v>
-      </c>
-      <c r="F79" s="1"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
+        <v>7792.51</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G79" s="2">
+        <v>41533</v>
+      </c>
+      <c r="H79" s="2">
+        <v>41536</v>
+      </c>
       <c r="I79" s="116">
-        <v>41542</v>
+        <v>41541</v>
       </c>
       <c r="J79" s="113" t="s">
         <v>23</v>
@@ -6381,26 +6420,20 @@
         <v>207</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E80" s="123">
-        <v>4489.5</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G80" s="2">
-        <v>41542</v>
-      </c>
-      <c r="H80" s="2">
-        <v>41545</v>
-      </c>
+        <v>10100</v>
+      </c>
+      <c r="F80" s="1"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
       <c r="I80" s="116">
         <v>41542</v>
       </c>
@@ -6410,7 +6443,7 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>86</v>
@@ -6419,24 +6452,24 @@
         <v>89</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>222</v>
+        <v>80</v>
       </c>
       <c r="E81" s="123">
-        <v>86.1</v>
+        <v>4489.5</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="G81" s="2">
-        <v>41570</v>
+        <v>41542</v>
       </c>
       <c r="H81" s="2">
-        <v>41573</v>
+        <v>41545</v>
       </c>
       <c r="I81" s="116">
-        <v>41570</v>
-      </c>
-      <c r="J81" t="s">
+        <v>41542</v>
+      </c>
+      <c r="J81" s="113" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6448,24 +6481,28 @@
         <v>86</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>180</v>
+        <v>89</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E82" s="123">
-        <v>1000</v>
+        <v>86.1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
+        <v>196</v>
+      </c>
+      <c r="G82" s="2">
+        <v>41570</v>
+      </c>
+      <c r="H82" s="2">
+        <v>41573</v>
+      </c>
       <c r="I82" s="116">
-        <v>41555</v>
-      </c>
-      <c r="J82" s="113" t="s">
-        <v>84</v>
+        <v>41570</v>
+      </c>
+      <c r="J82" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -6479,16 +6516,18 @@
         <v>180</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>32</v>
+        <v>221</v>
       </c>
       <c r="E83" s="123">
-        <v>6500</v>
-      </c>
-      <c r="F83" s="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="116">
-        <v>41565</v>
+        <v>41555</v>
       </c>
       <c r="J83" s="113" t="s">
         <v>84</v>
@@ -6499,26 +6538,24 @@
         <v>208</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E84" s="123">
-        <v>5640</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>6500</v>
+      </c>
+      <c r="F84" s="1"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="116">
-        <v>41585</v>
-      </c>
-      <c r="J84" t="s">
+        <v>41565</v>
+      </c>
+      <c r="J84" s="113" t="s">
         <v>84</v>
       </c>
     </row>
@@ -6533,43 +6570,43 @@
         <v>149</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E85" s="123">
-        <v>6372</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>5640</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
-      <c r="I85" s="116"/>
+      <c r="I85" s="116">
+        <v>41585</v>
+      </c>
+      <c r="J85" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>183</v>
+        <v>33</v>
       </c>
       <c r="E86" s="123">
-        <v>9249.7800000000007</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>184</v>
-      </c>
+        <v>6372</v>
+      </c>
+      <c r="F86" s="1"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
-      <c r="I86" s="116">
-        <v>41557</v>
-      </c>
-      <c r="J86" s="113" t="s">
-        <v>23</v>
-      </c>
+      <c r="I86" s="116"/>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
@@ -6582,13 +6619,13 @@
         <v>182</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E87" s="123">
-        <v>610</v>
+        <v>9249.7800000000007</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -6613,12 +6650,19 @@
         <v>185</v>
       </c>
       <c r="E88" s="123">
-        <v>1420.86</v>
-      </c>
-      <c r="F88" s="1"/>
+        <v>610</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
-      <c r="I88" s="116"/>
+      <c r="I88" s="116">
+        <v>41557</v>
+      </c>
+      <c r="J88" s="113" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="1" t="s">
@@ -6631,22 +6675,15 @@
         <v>182</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E89" s="123">
-        <v>790</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>188</v>
-      </c>
+        <v>1420.86</v>
+      </c>
+      <c r="F89" s="1"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
-      <c r="I89" s="116">
-        <v>41557</v>
-      </c>
-      <c r="J89" s="113" t="s">
-        <v>23</v>
-      </c>
+      <c r="I89" s="116"/>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
@@ -6662,12 +6699,19 @@
         <v>187</v>
       </c>
       <c r="E90" s="123">
-        <v>1841.26</v>
-      </c>
-      <c r="F90" s="1"/>
+        <v>790</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
-      <c r="I90" s="116"/>
+      <c r="I90" s="116">
+        <v>41557</v>
+      </c>
+      <c r="J90" s="113" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="1" t="s">
@@ -6680,22 +6724,15 @@
         <v>182</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E91" s="123">
-        <v>12076.41</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>190</v>
-      </c>
+        <v>1841.26</v>
+      </c>
+      <c r="F91" s="1"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
-      <c r="I91" s="116">
-        <v>41557</v>
-      </c>
-      <c r="J91" s="113" t="s">
-        <v>23</v>
-      </c>
+      <c r="I91" s="116"/>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="1" t="s">
@@ -6705,27 +6742,23 @@
         <v>86</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>89</v>
+        <v>182</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="E92" s="123">
-        <v>290.98</v>
+        <v>12076.41</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G92" s="2">
-        <v>41571</v>
-      </c>
-      <c r="H92" s="2">
-        <v>41574</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
       <c r="I92" s="116">
-        <v>41571</v>
-      </c>
-      <c r="J92" t="s">
+        <v>41557</v>
+      </c>
+      <c r="J92" s="113" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6737,28 +6770,19 @@
         <v>86</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>89</v>
+        <v>268</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>236</v>
+        <v>269</v>
       </c>
       <c r="E93" s="123">
-        <v>888</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G93" s="2">
-        <v>41583</v>
-      </c>
-      <c r="H93" s="2">
-        <v>41586</v>
-      </c>
+        <v>-2500</v>
+      </c>
+      <c r="F93" s="1"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
       <c r="I93" s="116">
-        <v>41586</v>
-      </c>
-      <c r="J93" t="s">
-        <v>23</v>
+        <v>41607</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -6772,22 +6796,22 @@
         <v>89</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="E94" s="123">
-        <v>367.84</v>
+        <v>290.98</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="G94" s="2">
-        <v>41585</v>
+        <v>41571</v>
       </c>
       <c r="H94" s="2">
-        <v>41588</v>
+        <v>41574</v>
       </c>
       <c r="I94" s="116">
-        <v>41586</v>
+        <v>41571</v>
       </c>
       <c r="J94" t="s">
         <v>23</v>
@@ -6804,22 +6828,22 @@
         <v>89</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E95" s="123">
-        <v>760.18</v>
+        <v>888</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G95" s="2">
-        <v>41591</v>
+        <v>41583</v>
       </c>
       <c r="H95" s="2">
-        <v>41594</v>
+        <v>41586</v>
       </c>
       <c r="I95" s="116">
-        <v>41595</v>
+        <v>41586</v>
       </c>
       <c r="J95" t="s">
         <v>23</v>
@@ -6833,21 +6857,25 @@
         <v>86</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>242</v>
+        <v>89</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E96" s="123">
-        <v>929.88</v>
+        <v>367.84</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
+        <v>237</v>
+      </c>
+      <c r="G96" s="2">
+        <v>41585</v>
+      </c>
+      <c r="H96" s="2">
+        <v>41588</v>
+      </c>
       <c r="I96" s="116">
-        <v>41592</v>
+        <v>41586</v>
       </c>
       <c r="J96" t="s">
         <v>23</v>
@@ -6864,22 +6892,22 @@
         <v>89</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="E97" s="123">
-        <v>104.7</v>
+        <v>760.18</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G97" s="2">
-        <v>41596</v>
+        <v>41591</v>
       </c>
       <c r="H97" s="2">
-        <v>41599</v>
+        <v>41594</v>
       </c>
       <c r="I97" s="116">
-        <v>41596</v>
+        <v>41595</v>
       </c>
       <c r="J97" t="s">
         <v>23</v>
@@ -6893,25 +6921,21 @@
         <v>86</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E98" s="123">
-        <v>120</v>
+        <v>929.88</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G98" s="2">
-        <v>41598</v>
-      </c>
-      <c r="H98" s="2">
-        <v>41601</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
       <c r="I98" s="116">
-        <v>41599</v>
+        <v>41592</v>
       </c>
       <c r="J98" t="s">
         <v>23</v>
@@ -6925,25 +6949,25 @@
         <v>86</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>182</v>
+        <v>89</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>264</v>
+        <v>14</v>
       </c>
       <c r="E99" s="123">
-        <v>960.45</v>
+        <v>104.7</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="G99" s="2">
-        <v>41600</v>
+        <v>41596</v>
       </c>
       <c r="H99" s="2">
-        <v>41600</v>
+        <v>41599</v>
       </c>
       <c r="I99" s="116">
-        <v>41605</v>
+        <v>41596</v>
       </c>
       <c r="J99" t="s">
         <v>23</v>
@@ -6951,31 +6975,31 @@
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>89</v>
+        <v>182</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>22</v>
+        <v>248</v>
       </c>
       <c r="E100" s="123">
-        <v>312.33</v>
+        <v>120</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="G100" s="2">
-        <v>41582</v>
+        <v>41598</v>
       </c>
       <c r="H100" s="2">
-        <v>41585</v>
+        <v>41601</v>
       </c>
       <c r="I100" s="116">
-        <v>41582</v>
+        <v>41599</v>
       </c>
       <c r="J100" t="s">
         <v>23</v>
@@ -6983,33 +7007,39 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="E101" s="123">
-        <v>200</v>
-      </c>
-      <c r="F101" s="1"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
+        <v>960.45</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G101" s="2">
+        <v>41600</v>
+      </c>
+      <c r="H101" s="2">
+        <v>41600</v>
+      </c>
       <c r="I101" s="116">
-        <v>41585</v>
+        <v>41605</v>
       </c>
       <c r="J101" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>86</v>
@@ -7021,19 +7051,19 @@
         <v>22</v>
       </c>
       <c r="E102" s="123">
-        <v>60.89</v>
+        <v>312.33</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="G102" s="2">
-        <v>41570</v>
+        <v>41582</v>
       </c>
       <c r="H102" s="2">
-        <v>41573</v>
+        <v>41585</v>
       </c>
       <c r="I102" s="116">
-        <v>41570</v>
+        <v>41582</v>
       </c>
       <c r="J102" t="s">
         <v>23</v>
@@ -7041,34 +7071,28 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>22</v>
+        <v>230</v>
       </c>
       <c r="E103" s="123">
-        <v>84.89</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G103" s="2">
-        <v>41577</v>
-      </c>
-      <c r="H103" s="2">
-        <v>41580</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F103" s="1"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
       <c r="I103" s="116">
-        <v>41577</v>
+        <v>41585</v>
       </c>
       <c r="J103" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -7076,25 +7100,31 @@
         <v>210</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>227</v>
+        <v>22</v>
       </c>
       <c r="E104" s="123">
-        <v>180</v>
-      </c>
-      <c r="F104" s="1"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
+        <v>60.89</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G104" s="2">
+        <v>41570</v>
+      </c>
+      <c r="H104" s="2">
+        <v>41573</v>
+      </c>
       <c r="I104" s="116">
-        <v>41585</v>
+        <v>41570</v>
       </c>
       <c r="J104" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -7105,19 +7135,25 @@
         <v>86</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>255</v>
+        <v>89</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>256</v>
+        <v>22</v>
       </c>
       <c r="E105" s="123">
-        <v>1323</v>
-      </c>
-      <c r="F105" s="1"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
+        <v>84.89</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G105" s="2">
+        <v>41577</v>
+      </c>
+      <c r="H105" s="2">
+        <v>41580</v>
+      </c>
       <c r="I105" s="116">
-        <v>41602</v>
+        <v>41577</v>
       </c>
       <c r="J105" t="s">
         <v>23</v>
@@ -7128,21 +7164,26 @@
         <v>210</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>255</v>
+        <v>149</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="E106" s="123">
-        <v>3086</v>
+        <v>180</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
-      <c r="I106" s="116"/>
+      <c r="I106" s="116">
+        <v>41585</v>
+      </c>
+      <c r="J106" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1" t="s">
@@ -7152,19 +7193,19 @@
         <v>86</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E107" s="123">
-        <v>8555</v>
+        <v>1323</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="116">
-        <v>41582</v>
+        <v>41602</v>
       </c>
       <c r="J107" t="s">
         <v>23</v>
@@ -7178,13 +7219,13 @@
         <v>86</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E108" s="123">
-        <v>8555</v>
+        <v>3086</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="2"/>
@@ -7193,31 +7234,25 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>89</v>
+        <v>257</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="E109" s="123">
-        <v>5326</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G109" s="2">
-        <v>41570</v>
-      </c>
-      <c r="H109" s="2">
-        <v>41573</v>
-      </c>
+        <v>8555</v>
+      </c>
+      <c r="F109" s="1"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
       <c r="I109" s="116">
-        <v>41570</v>
+        <v>41582</v>
       </c>
       <c r="J109" t="s">
         <v>23</v>
@@ -7225,60 +7260,55 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>89</v>
+        <v>257</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="E110" s="123">
-        <v>93.52</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G110" s="2">
-        <v>41571</v>
-      </c>
-      <c r="H110" s="2">
-        <v>41574</v>
-      </c>
-      <c r="I110" s="116">
-        <v>41571</v>
-      </c>
-      <c r="J110" t="s">
-        <v>23</v>
-      </c>
+        <v>8555</v>
+      </c>
+      <c r="F110" s="1"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="116"/>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>232</v>
+        <v>104</v>
       </c>
       <c r="E111" s="123">
-        <v>4400</v>
-      </c>
-      <c r="F111" s="1"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
+        <v>5326</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G111" s="2">
+        <v>41570</v>
+      </c>
+      <c r="H111" s="2">
+        <v>41573</v>
+      </c>
       <c r="I111" s="116">
-        <v>41585</v>
+        <v>41570</v>
       </c>
       <c r="J111" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -7292,22 +7322,22 @@
         <v>89</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="E112" s="123">
-        <v>227.67</v>
+        <v>93.52</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="G112" s="2">
-        <v>41582</v>
+        <v>41571</v>
       </c>
       <c r="H112" s="2">
-        <v>41585</v>
+        <v>41574</v>
       </c>
       <c r="I112" s="116">
-        <v>41582</v>
+        <v>41571</v>
       </c>
       <c r="J112" t="s">
         <v>23</v>
@@ -7318,31 +7348,25 @@
         <v>211</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>104</v>
+        <v>232</v>
       </c>
       <c r="E113" s="123">
-        <v>1214.3399999999999</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G113" s="2">
-        <v>41582</v>
-      </c>
-      <c r="H113" s="2">
+        <v>4400</v>
+      </c>
+      <c r="F113" s="1"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="116">
         <v>41585</v>
       </c>
-      <c r="I113" s="116">
-        <v>41582</v>
-      </c>
       <c r="J113" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -7350,25 +7374,31 @@
         <v>211</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>228</v>
+        <v>48</v>
       </c>
       <c r="E114" s="123">
-        <v>90</v>
-      </c>
-      <c r="F114" s="1"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
+        <v>227.67</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G114" s="2">
+        <v>41582</v>
+      </c>
+      <c r="H114" s="2">
+        <v>41585</v>
+      </c>
       <c r="I114" s="116">
-        <v>41585</v>
+        <v>41582</v>
       </c>
       <c r="J114" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -7376,25 +7406,31 @@
         <v>211</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>229</v>
+        <v>104</v>
       </c>
       <c r="E115" s="123">
-        <v>120</v>
-      </c>
-      <c r="F115" s="1"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
+        <v>1214.3399999999999</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G115" s="2">
+        <v>41582</v>
+      </c>
+      <c r="H115" s="2">
+        <v>41585</v>
+      </c>
       <c r="I115" s="116">
-        <v>41585</v>
+        <v>41582</v>
       </c>
       <c r="J115" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -7402,31 +7438,25 @@
         <v>211</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="E116" s="123">
-        <v>257.45999999999998</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G116" s="2">
-        <v>41583</v>
-      </c>
-      <c r="H116" s="2">
-        <v>41586</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F116" s="1"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
       <c r="I116" s="116">
-        <v>41586</v>
+        <v>41585</v>
       </c>
       <c r="J116" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -7434,103 +7464,161 @@
         <v>211</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E117" s="123">
+        <v>120</v>
+      </c>
+      <c r="F117" s="1"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="116">
+        <v>41585</v>
+      </c>
+      <c r="J117" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D118" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E118" s="123">
+        <v>257.45999999999998</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G118" s="2">
+        <v>41583</v>
+      </c>
+      <c r="H118" s="2">
+        <v>41586</v>
+      </c>
+      <c r="I118" s="116">
+        <v>41586</v>
+      </c>
+      <c r="J118" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E117" s="123">
+      <c r="E119" s="123">
         <v>272.37</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="G117" s="2">
+      <c r="G119" s="2">
         <v>41585</v>
       </c>
-      <c r="H117" s="2">
+      <c r="H119" s="2">
         <v>41588</v>
       </c>
-      <c r="I117" s="116">
+      <c r="I119" s="116">
         <v>41586</v>
       </c>
-      <c r="J117" t="s">
+      <c r="J119" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="123"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="116"/>
-    </row>
-    <row r="119" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A119" s="44" t="s">
+    <row r="120" spans="1:10">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="123"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="116"/>
+    </row>
+    <row r="121" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A121" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B119" s="44"/>
-      <c r="C119" s="44"/>
-      <c r="D119" s="44"/>
-      <c r="E119" s="124">
+      <c r="B121" s="44"/>
+      <c r="C121" s="44"/>
+      <c r="D121" s="44"/>
+      <c r="E121" s="124">
         <f>SUBTOTAL(109,[Kwota])</f>
-        <v>227001</v>
-      </c>
-      <c r="F119" s="44"/>
-      <c r="G119" s="44"/>
-      <c r="H119" s="44"/>
-      <c r="I119" s="117"/>
-      <c r="J119" s="114">
+        <v>225232.85000000003</v>
+      </c>
+      <c r="F121" s="44"/>
+      <c r="G121" s="44"/>
+      <c r="H121" s="44"/>
+      <c r="I121" s="117"/>
+      <c r="J121" s="114">
         <f>SUBTOTAL(103,[Konto])</f>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="15.75" thickTop="1"/>
-    <row r="127" spans="1:10">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
-      <c r="E127" s="122"/>
-      <c r="F127" s="1"/>
-      <c r="G127" s="1"/>
-      <c r="H127" s="1"/>
-      <c r="I127" s="118"/>
-      <c r="J127" s="110"/>
-    </row>
-    <row r="128" spans="1:10">
-      <c r="C128" s="109"/>
-      <c r="D128" s="109"/>
-    </row>
-    <row r="144" spans="1:10">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
-      <c r="C144" s="1"/>
-      <c r="D144" s="1"/>
-      <c r="E144" s="122"/>
-      <c r="F144" s="1"/>
-      <c r="G144" s="1"/>
-      <c r="H144" s="1"/>
-      <c r="I144" s="118"/>
-      <c r="J144" s="110"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="129" spans="1:10">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="122"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="118"/>
+      <c r="J129" s="110"/>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="C130" s="109"/>
+      <c r="D130" s="109"/>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="122"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="118"/>
+      <c r="J146" s="110"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B120:B127 B102 B114:B115 B111 B28:B81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122:B129 B104 B116:B117 B113 B29:B82">
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A120:A127">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A122:A129">
       <formula1>$M$4:$M$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A118">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A120">
       <formula1>$M$3:$M$19</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>